<commit_message>
Update counties spreadsheet and stats
</commit_message>
<xml_diff>
--- a/Locations/CountyStats.xlsx
+++ b/Locations/CountyStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\Rainfall\DQ_Checks\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65E52B9-90B6-4B50-BF1B-316512463FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF6D1D3-9D2F-410B-A927-BEDB0F4B7CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B7A8E3D-5389-431E-9666-1FDD2E742F2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9FC44E90-B471-4E48-9C23-0D2D4F7032F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -561,18 +561,18 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -888,115 +888,114 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85C856D-289A-4E14-B0C5-DA0812985737}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C4A73A-736C-4D01-9A09-14E5731A8B3B}">
   <dimension ref="A1:P139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.140625" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="K1" s="6" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="K1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="9" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="K2" s="2" t="s">
+      <c r="I2" s="8"/>
+      <c r="K2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="9" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="9"/>
+      <c r="P2" s="8"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="12"/>
-      <c r="K3" s="10" t="s">
+      <c r="J3" s="11"/>
+      <c r="K3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="10"/>
-      <c r="O3" s="11" t="s">
+      <c r="N3" s="9"/>
+      <c r="O3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1013,10 +1012,10 @@
       <c r="F4">
         <v>9</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="12">
         <v>1</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="12">
         <v>0</v>
       </c>
       <c r="K4">
@@ -1025,10 +1024,10 @@
       <c r="M4">
         <v>823</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4" s="12">
         <v>1</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4" s="12">
         <v>0</v>
       </c>
     </row>
@@ -1045,10 +1044,10 @@
       <c r="F5">
         <v>113</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="12">
         <v>0.27433628318584069</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="12">
         <v>0.72566371681415931</v>
       </c>
       <c r="K5">
@@ -1060,10 +1059,10 @@
       <c r="M5">
         <v>7725</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5" s="12">
         <v>0.33721682847896439</v>
       </c>
-      <c r="P5" s="1">
+      <c r="P5" s="12">
         <v>0.66278317152103561</v>
       </c>
     </row>
@@ -1077,10 +1076,10 @@
       <c r="F6">
         <v>3</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="12">
         <v>1</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="12">
         <v>0</v>
       </c>
       <c r="K6">
@@ -1089,10 +1088,10 @@
       <c r="M6">
         <v>229</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="12">
         <v>1</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="12">
         <v>0</v>
       </c>
     </row>
@@ -1101,34 +1100,34 @@
         <v>10</v>
       </c>
       <c r="D7">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="E7">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="F7">
         <v>113</v>
       </c>
-      <c r="H7" s="1">
-        <v>0.44247787610619471</v>
-      </c>
-      <c r="I7" s="1">
-        <v>0.55752212389380529</v>
+      <c r="H7" s="12">
+        <v>0.62831858407079644</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0.37168141592920356</v>
       </c>
       <c r="K7">
-        <v>4429</v>
+        <v>6555</v>
       </c>
       <c r="L7">
-        <v>3784</v>
+        <v>1658</v>
       </c>
       <c r="M7">
         <v>8213</v>
       </c>
-      <c r="O7" s="1">
-        <v>0.53926701570680624</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0.4607329842931937</v>
+      <c r="O7" s="12">
+        <v>0.79812492390113232</v>
+      </c>
+      <c r="P7" s="12">
+        <v>0.20187507609886765</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1144,10 +1143,10 @@
       <c r="F8">
         <v>8</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="12">
         <v>0.875</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="12">
         <v>0.125</v>
       </c>
       <c r="K8">
@@ -1159,10 +1158,10 @@
       <c r="M8">
         <v>639</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="12">
         <v>0.83098591549295775</v>
       </c>
-      <c r="P8" s="1">
+      <c r="P8" s="12">
         <v>0.16901408450704225</v>
       </c>
     </row>
@@ -1173,37 +1172,37 @@
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="E9" s="13">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="F9" s="13">
         <v>246</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="14">
-        <v>0.4065040650406504</v>
+        <v>0.491869918699187</v>
       </c>
       <c r="I9" s="14">
-        <v>0.5934959349593496</v>
+        <v>0.50813008130081305</v>
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="13">
-        <v>8617</v>
+        <v>10743</v>
       </c>
       <c r="L9" s="13">
-        <v>9012</v>
+        <v>6886</v>
       </c>
       <c r="M9" s="13">
         <v>17629</v>
       </c>
       <c r="N9" s="13"/>
       <c r="O9" s="14">
-        <v>0.48879686879573431</v>
+        <v>0.6093936127970957</v>
       </c>
       <c r="P9" s="14">
-        <v>0.51120313120426575</v>
+        <v>0.3906063872029043</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1222,10 +1221,10 @@
       <c r="F10">
         <v>413</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="12">
         <v>0.60290556900726389</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="12">
         <v>0.39709443099273606</v>
       </c>
       <c r="K10">
@@ -1237,10 +1236,10 @@
       <c r="M10">
         <v>32229</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10" s="12">
         <v>0.69887368519035653</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10" s="12">
         <v>0.30112631480964347</v>
       </c>
     </row>
@@ -1257,10 +1256,10 @@
       <c r="F11">
         <v>782</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="12">
         <v>0.52685421994884907</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="12">
         <v>0.47314578005115088</v>
       </c>
       <c r="K11">
@@ -1272,10 +1271,10 @@
       <c r="M11">
         <v>60632</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="12">
         <v>0.63473083520253326</v>
       </c>
-      <c r="P11" s="1">
+      <c r="P11" s="12">
         <v>0.36526916479746668</v>
       </c>
     </row>
@@ -1292,10 +1291,10 @@
       <c r="F12">
         <v>574</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="12">
         <v>0.43205574912891986</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="12">
         <v>0.56794425087108014</v>
       </c>
       <c r="K12">
@@ -1307,10 +1306,10 @@
       <c r="M12">
         <v>43861</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O12" s="12">
         <v>0.50735277353457509</v>
       </c>
-      <c r="P12" s="1">
+      <c r="P12" s="12">
         <v>0.49264722646542486</v>
       </c>
     </row>
@@ -1327,10 +1326,10 @@
       <c r="F13">
         <v>567</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="12">
         <v>0.57319223985890655</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="12">
         <v>0.42680776014109345</v>
       </c>
       <c r="K13">
@@ -1342,10 +1341,10 @@
       <c r="M13">
         <v>47683</v>
       </c>
-      <c r="O13" s="1">
+      <c r="O13" s="12">
         <v>0.68026340624541237</v>
       </c>
-      <c r="P13" s="1">
+      <c r="P13" s="12">
         <v>0.31973659375458757</v>
       </c>
     </row>
@@ -1354,34 +1353,34 @@
         <v>18</v>
       </c>
       <c r="D14">
-        <v>702</v>
+        <v>755</v>
       </c>
       <c r="E14">
-        <v>405</v>
+        <v>352</v>
       </c>
       <c r="F14">
         <v>1107</v>
       </c>
-      <c r="H14" s="1">
-        <v>0.63414634146341464</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0.36585365853658536</v>
+      <c r="H14" s="12">
+        <v>0.68202348690153569</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0.31797651309846431</v>
       </c>
       <c r="K14">
-        <v>65859</v>
+        <v>71424</v>
       </c>
       <c r="L14">
-        <v>26500</v>
+        <v>20935</v>
       </c>
       <c r="M14">
         <v>92359</v>
       </c>
-      <c r="O14" s="1">
-        <v>0.7130761485074546</v>
-      </c>
-      <c r="P14" s="1">
-        <v>0.2869238514925454</v>
+      <c r="O14" s="12">
+        <v>0.77333015732088917</v>
+      </c>
+      <c r="P14" s="12">
+        <v>0.22666984267911086</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1397,10 +1396,10 @@
       <c r="F15">
         <v>973</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="12">
         <v>0.58992805755395683</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="12">
         <v>0.41007194244604317</v>
       </c>
       <c r="K15">
@@ -1412,10 +1411,10 @@
       <c r="M15">
         <v>74376</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15" s="12">
         <v>0.69238732924599333</v>
       </c>
-      <c r="P15" s="1">
+      <c r="P15" s="12">
         <v>0.30761267075400667</v>
       </c>
     </row>
@@ -1432,10 +1431,10 @@
       <c r="F16">
         <v>1084</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="12">
         <v>0.70756457564575648</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="12">
         <v>0.29243542435424352</v>
       </c>
       <c r="K16">
@@ -1447,10 +1446,10 @@
       <c r="M16">
         <v>82480</v>
       </c>
-      <c r="O16" s="1">
+      <c r="O16" s="12">
         <v>0.79620514064015524</v>
       </c>
-      <c r="P16" s="1">
+      <c r="P16" s="12">
         <v>0.20379485935984482</v>
       </c>
     </row>
@@ -1459,34 +1458,34 @@
         <v>21</v>
       </c>
       <c r="D17">
-        <v>715</v>
+        <v>722</v>
       </c>
       <c r="E17">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="F17">
         <v>1225</v>
       </c>
-      <c r="H17" s="1">
-        <v>0.58367346938775511</v>
-      </c>
-      <c r="I17" s="1">
-        <v>0.41632653061224489</v>
+      <c r="H17" s="12">
+        <v>0.58938775510204078</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0.41061224489795917</v>
       </c>
       <c r="K17">
-        <v>67592</v>
+        <v>68228</v>
       </c>
       <c r="L17">
-        <v>35171</v>
+        <v>34535</v>
       </c>
       <c r="M17">
         <v>102763</v>
       </c>
-      <c r="O17" s="1">
-        <v>0.65774646516742408</v>
-      </c>
-      <c r="P17" s="1">
-        <v>0.34225353483257592</v>
+      <c r="O17" s="12">
+        <v>0.66393546315308039</v>
+      </c>
+      <c r="P17" s="12">
+        <v>0.33606453684691961</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
@@ -1494,34 +1493,34 @@
         <v>22</v>
       </c>
       <c r="D18">
-        <v>1355</v>
+        <v>1465</v>
       </c>
       <c r="E18">
-        <v>1196</v>
+        <v>1086</v>
       </c>
       <c r="F18">
         <v>2551</v>
       </c>
-      <c r="H18" s="1">
-        <v>0.53116424931399453</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0.46883575068600547</v>
+      <c r="H18" s="12">
+        <v>0.57428459427675427</v>
+      </c>
+      <c r="I18" s="12">
+        <v>0.42571540572324579</v>
       </c>
       <c r="K18">
-        <v>122823</v>
+        <v>132606</v>
       </c>
       <c r="L18">
-        <v>71398</v>
+        <v>61615</v>
       </c>
       <c r="M18">
         <v>194221</v>
       </c>
-      <c r="O18" s="1">
-        <v>0.6323878468342764</v>
-      </c>
-      <c r="P18" s="1">
-        <v>0.3676121531657236</v>
+      <c r="O18" s="12">
+        <v>0.68275830111059055</v>
+      </c>
+      <c r="P18" s="12">
+        <v>0.31724169888940951</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -1529,34 +1528,34 @@
         <v>23</v>
       </c>
       <c r="D19">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="E19">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F19">
         <v>955</v>
       </c>
-      <c r="H19" s="1">
-        <v>0.406282722513089</v>
-      </c>
-      <c r="I19" s="1">
-        <v>0.59371727748691094</v>
+      <c r="H19" s="12">
+        <v>0.40942408376963352</v>
+      </c>
+      <c r="I19" s="12">
+        <v>0.59057591623036654</v>
       </c>
       <c r="K19">
-        <v>35738</v>
+        <v>35984</v>
       </c>
       <c r="L19">
-        <v>35241</v>
+        <v>34995</v>
       </c>
       <c r="M19">
         <v>70979</v>
       </c>
-      <c r="O19" s="1">
-        <v>0.50350103551754744</v>
-      </c>
-      <c r="P19" s="1">
-        <v>0.49649896448245256</v>
+      <c r="O19" s="12">
+        <v>0.50696684934980774</v>
+      </c>
+      <c r="P19" s="12">
+        <v>0.49303315065019232</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
@@ -1564,34 +1563,34 @@
         <v>24</v>
       </c>
       <c r="D20">
-        <v>449</v>
+        <v>497</v>
       </c>
       <c r="E20">
-        <v>214</v>
+        <v>166</v>
       </c>
       <c r="F20">
         <v>663</v>
       </c>
-      <c r="H20" s="1">
-        <v>0.6772247360482655</v>
-      </c>
-      <c r="I20" s="1">
-        <v>0.32277526395173456</v>
+      <c r="H20" s="12">
+        <v>0.74962292609351433</v>
+      </c>
+      <c r="I20" s="12">
+        <v>0.25037707390648567</v>
       </c>
       <c r="K20">
-        <v>42050</v>
+        <v>45970</v>
       </c>
       <c r="L20">
-        <v>12812</v>
+        <v>8892</v>
       </c>
       <c r="M20">
         <v>54862</v>
       </c>
-      <c r="O20" s="1">
-        <v>0.7664685939265794</v>
-      </c>
-      <c r="P20" s="1">
-        <v>0.23353140607342057</v>
+      <c r="O20" s="12">
+        <v>0.8379206007801393</v>
+      </c>
+      <c r="P20" s="12">
+        <v>0.16207939921986075</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
@@ -1599,34 +1598,34 @@
         <v>25</v>
       </c>
       <c r="D21">
-        <v>657</v>
+        <v>663</v>
       </c>
       <c r="E21">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="F21">
         <v>1290</v>
       </c>
-      <c r="H21" s="1">
-        <v>0.50930232558139532</v>
-      </c>
-      <c r="I21" s="1">
-        <v>0.49069767441860462</v>
+      <c r="H21" s="12">
+        <v>0.51395348837209298</v>
+      </c>
+      <c r="I21" s="12">
+        <v>0.48604651162790696</v>
       </c>
       <c r="K21">
-        <v>62830</v>
+        <v>63394</v>
       </c>
       <c r="L21">
-        <v>38653</v>
+        <v>38089</v>
       </c>
       <c r="M21">
         <v>101483</v>
       </c>
-      <c r="O21" s="1">
-        <v>0.61911847304474643</v>
-      </c>
-      <c r="P21" s="1">
-        <v>0.38088152695525357</v>
+      <c r="O21" s="12">
+        <v>0.62467605411743843</v>
+      </c>
+      <c r="P21" s="12">
+        <v>0.37532394588256163</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -1642,10 +1641,10 @@
       <c r="F22">
         <v>1179</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="12">
         <v>0.48854961832061067</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="12">
         <v>0.51145038167938928</v>
       </c>
       <c r="K22">
@@ -1657,10 +1656,10 @@
       <c r="M22">
         <v>95612</v>
       </c>
-      <c r="O22" s="1">
+      <c r="O22" s="12">
         <v>0.57047232564950001</v>
       </c>
-      <c r="P22" s="1">
+      <c r="P22" s="12">
         <v>0.42952767435049993</v>
       </c>
     </row>
@@ -1669,34 +1668,34 @@
         <v>27</v>
       </c>
       <c r="D23">
-        <v>702</v>
+        <v>711</v>
       </c>
       <c r="E23">
-        <v>1019</v>
+        <v>1010</v>
       </c>
       <c r="F23">
         <v>1721</v>
       </c>
-      <c r="H23" s="1">
-        <v>0.40790238233585124</v>
-      </c>
-      <c r="I23" s="1">
-        <v>0.5920976176641487</v>
+      <c r="H23" s="12">
+        <v>0.41313190005810574</v>
+      </c>
+      <c r="I23" s="12">
+        <v>0.58686809994189426</v>
       </c>
       <c r="K23">
-        <v>64115</v>
+        <v>64800</v>
       </c>
       <c r="L23">
-        <v>66956</v>
+        <v>66271</v>
       </c>
       <c r="M23">
         <v>131071</v>
       </c>
-      <c r="O23" s="1">
-        <v>0.48916236238374622</v>
-      </c>
-      <c r="P23" s="1">
-        <v>0.51083763761625378</v>
+      <c r="O23" s="12">
+        <v>0.4943885375102044</v>
+      </c>
+      <c r="P23" s="12">
+        <v>0.5056114624897956</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
@@ -1712,10 +1711,10 @@
       <c r="F24">
         <v>590</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="12">
         <v>0.4033898305084746</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24" s="12">
         <v>0.59661016949152545</v>
       </c>
       <c r="K24">
@@ -1727,10 +1726,10 @@
       <c r="M24">
         <v>44313</v>
       </c>
-      <c r="O24" s="1">
+      <c r="O24" s="12">
         <v>0.50544986798456437</v>
       </c>
-      <c r="P24" s="1">
+      <c r="P24" s="12">
         <v>0.49455013201543563</v>
       </c>
     </row>
@@ -1747,10 +1746,10 @@
       <c r="F25">
         <v>1002</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="12">
         <v>0.46107784431137727</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="12">
         <v>0.53892215568862278</v>
       </c>
       <c r="K25">
@@ -1762,10 +1761,10 @@
       <c r="M25">
         <v>79700</v>
       </c>
-      <c r="O25" s="1">
+      <c r="O25" s="12">
         <v>0.55879548306148052</v>
       </c>
-      <c r="P25" s="1">
+      <c r="P25" s="12">
         <v>0.44120451693851948</v>
       </c>
     </row>
@@ -1782,10 +1781,10 @@
       <c r="F26">
         <v>137</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26" s="12">
         <v>0.55474452554744524</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26" s="12">
         <v>0.44525547445255476</v>
       </c>
       <c r="K26">
@@ -1797,10 +1796,10 @@
       <c r="M26">
         <v>10380</v>
       </c>
-      <c r="O26" s="1">
+      <c r="O26" s="12">
         <v>0.68217726396917144</v>
       </c>
-      <c r="P26" s="1">
+      <c r="P26" s="12">
         <v>0.3178227360308285</v>
       </c>
     </row>
@@ -1817,10 +1816,10 @@
       <c r="F27">
         <v>251</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27" s="12">
         <v>0.68127490039840632</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27" s="12">
         <v>0.31872509960159362</v>
       </c>
       <c r="K27">
@@ -1832,10 +1831,10 @@
       <c r="M27">
         <v>19731</v>
       </c>
-      <c r="O27" s="1">
+      <c r="O27" s="12">
         <v>0.80011149967056916</v>
       </c>
-      <c r="P27" s="1">
+      <c r="P27" s="12">
         <v>0.19988850032943084</v>
       </c>
     </row>
@@ -1844,34 +1843,34 @@
         <v>32</v>
       </c>
       <c r="D28">
-        <v>925</v>
+        <v>933</v>
       </c>
       <c r="E28">
-        <v>1299</v>
+        <v>1291</v>
       </c>
       <c r="F28">
         <v>2224</v>
       </c>
-      <c r="H28" s="1">
-        <v>0.41591726618705038</v>
-      </c>
-      <c r="I28" s="1">
-        <v>0.58408273381294962</v>
+      <c r="H28" s="12">
+        <v>0.41951438848920863</v>
+      </c>
+      <c r="I28" s="12">
+        <v>0.58048561151079137</v>
       </c>
       <c r="K28">
-        <v>86729</v>
+        <v>87517</v>
       </c>
       <c r="L28">
-        <v>84605</v>
+        <v>83817</v>
       </c>
       <c r="M28">
         <v>171334</v>
       </c>
-      <c r="O28" s="1">
-        <v>0.50619841946140287</v>
-      </c>
-      <c r="P28" s="1">
-        <v>0.49380158053859713</v>
+      <c r="O28" s="12">
+        <v>0.51079762335555112</v>
+      </c>
+      <c r="P28" s="12">
+        <v>0.48920237664444888</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
@@ -1879,34 +1878,34 @@
         <v>33</v>
       </c>
       <c r="D29">
-        <v>1979</v>
+        <v>1983</v>
       </c>
       <c r="E29">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="F29">
         <v>3110</v>
       </c>
-      <c r="H29" s="1">
-        <v>0.63633440514469453</v>
-      </c>
-      <c r="I29" s="1">
-        <v>0.36366559485530547</v>
+      <c r="H29" s="12">
+        <v>0.63762057877813505</v>
+      </c>
+      <c r="I29" s="12">
+        <v>0.36237942122186495</v>
       </c>
       <c r="K29">
-        <v>190420</v>
+        <v>190767</v>
       </c>
       <c r="L29">
-        <v>78009</v>
+        <v>77662</v>
       </c>
       <c r="M29">
         <v>268429</v>
       </c>
-      <c r="O29" s="1">
-        <v>0.70938683972298078</v>
-      </c>
-      <c r="P29" s="1">
-        <v>0.29061316027701922</v>
+      <c r="O29" s="12">
+        <v>0.71067954654675913</v>
+      </c>
+      <c r="P29" s="12">
+        <v>0.28932045345324087</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
@@ -1922,10 +1921,10 @@
       <c r="F30">
         <v>498</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30" s="12">
         <v>0.51405622489959835</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30" s="12">
         <v>0.4859437751004016</v>
       </c>
       <c r="K30">
@@ -1937,10 +1936,10 @@
       <c r="M30">
         <v>40740</v>
       </c>
-      <c r="O30" s="1">
+      <c r="O30" s="12">
         <v>0.62032400589101622</v>
       </c>
-      <c r="P30" s="1">
+      <c r="P30" s="12">
         <v>0.37967599410898378</v>
       </c>
     </row>
@@ -1957,10 +1956,10 @@
       <c r="F31">
         <v>1037</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31" s="12">
         <v>0.70395371263259399</v>
       </c>
-      <c r="I31" s="1">
+      <c r="I31" s="12">
         <v>0.29604628736740596</v>
       </c>
       <c r="K31">
@@ -1972,10 +1971,10 @@
       <c r="M31">
         <v>85136</v>
       </c>
-      <c r="O31" s="1">
+      <c r="O31" s="12">
         <v>0.81899548956962975</v>
       </c>
-      <c r="P31" s="1">
+      <c r="P31" s="12">
         <v>0.18100451043037022</v>
       </c>
     </row>
@@ -1992,10 +1991,10 @@
       <c r="F32">
         <v>527</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H32" s="12">
         <v>0.62618595825426948</v>
       </c>
-      <c r="I32" s="1">
+      <c r="I32" s="12">
         <v>0.37381404174573057</v>
       </c>
       <c r="K32">
@@ -2007,10 +2006,10 @@
       <c r="M32">
         <v>44827</v>
       </c>
-      <c r="O32" s="1">
+      <c r="O32" s="12">
         <v>0.75512525933031427</v>
       </c>
-      <c r="P32" s="1">
+      <c r="P32" s="12">
         <v>0.24487474066968568</v>
       </c>
     </row>
@@ -2027,10 +2026,10 @@
       <c r="F33">
         <v>1072</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H33" s="12">
         <v>0.54570895522388063</v>
       </c>
-      <c r="I33" s="1">
+      <c r="I33" s="12">
         <v>0.45429104477611942</v>
       </c>
       <c r="K33">
@@ -2042,10 +2041,10 @@
       <c r="M33">
         <v>76409</v>
       </c>
-      <c r="O33" s="1">
+      <c r="O33" s="12">
         <v>0.66396628669397584</v>
       </c>
-      <c r="P33" s="1">
+      <c r="P33" s="12">
         <v>0.33603371330602416</v>
       </c>
     </row>
@@ -2062,10 +2061,10 @@
       <c r="F34">
         <v>1141</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H34" s="12">
         <v>0.51621384750219101</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I34" s="12">
         <v>0.48378615249780893</v>
       </c>
       <c r="K34">
@@ -2077,10 +2076,10 @@
       <c r="M34">
         <v>87438</v>
       </c>
-      <c r="O34" s="1">
+      <c r="O34" s="12">
         <v>0.61524737528305773</v>
       </c>
-      <c r="P34" s="1">
+      <c r="P34" s="12">
         <v>0.38475262471694227</v>
       </c>
     </row>
@@ -2097,10 +2096,10 @@
       <c r="F35">
         <v>784</v>
       </c>
-      <c r="H35" s="1">
+      <c r="H35" s="12">
         <v>0.5535714285714286</v>
       </c>
-      <c r="I35" s="1">
+      <c r="I35" s="12">
         <v>0.44642857142857145</v>
       </c>
       <c r="K35">
@@ -2112,10 +2111,10 @@
       <c r="M35">
         <v>62591</v>
       </c>
-      <c r="O35" s="1">
+      <c r="O35" s="12">
         <v>0.64426195459411095</v>
       </c>
-      <c r="P35" s="1">
+      <c r="P35" s="12">
         <v>0.35573804540588905</v>
       </c>
     </row>
@@ -2132,10 +2131,10 @@
       <c r="F36">
         <v>821</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H36" s="12">
         <v>0.66382460414129107</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I36" s="12">
         <v>0.33617539585870887</v>
       </c>
       <c r="K36">
@@ -2147,10 +2146,10 @@
       <c r="M36">
         <v>64835</v>
       </c>
-      <c r="O36" s="1">
+      <c r="O36" s="12">
         <v>0.79131641860106428</v>
       </c>
-      <c r="P36" s="1">
+      <c r="P36" s="12">
         <v>0.20868358139893575</v>
       </c>
     </row>
@@ -2167,10 +2166,10 @@
       <c r="F37">
         <v>686</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H37" s="12">
         <v>0.58746355685131191</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I37" s="12">
         <v>0.41253644314868804</v>
       </c>
       <c r="K37">
@@ -2182,10 +2181,10 @@
       <c r="M37">
         <v>57919</v>
       </c>
-      <c r="O37" s="1">
+      <c r="O37" s="12">
         <v>0.67293979523127123</v>
       </c>
-      <c r="P37" s="1">
+      <c r="P37" s="12">
         <v>0.32706020476872877</v>
       </c>
     </row>
@@ -2194,19 +2193,19 @@
         <v>42</v>
       </c>
       <c r="D38">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E38">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="F38">
         <v>760</v>
       </c>
-      <c r="H38" s="1">
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="I38" s="1">
-        <v>0.57499999999999996</v>
+      <c r="H38" s="12">
+        <v>0.42368421052631577</v>
+      </c>
+      <c r="I38" s="12">
+        <v>0.57631578947368423</v>
       </c>
       <c r="K38">
         <v>29719</v>
@@ -2217,10 +2216,10 @@
       <c r="M38">
         <v>55284</v>
       </c>
-      <c r="O38" s="1">
+      <c r="O38" s="12">
         <v>0.53756964040228639</v>
       </c>
-      <c r="P38" s="1">
+      <c r="P38" s="12">
         <v>0.46243035959771361</v>
       </c>
     </row>
@@ -2237,10 +2236,10 @@
       <c r="F39">
         <v>95</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H39" s="12">
         <v>0.61052631578947369</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I39" s="12">
         <v>0.38947368421052631</v>
       </c>
       <c r="K39">
@@ -2252,10 +2251,10 @@
       <c r="M39">
         <v>6706</v>
       </c>
-      <c r="O39" s="1">
+      <c r="O39" s="12">
         <v>0.69549657023560996</v>
       </c>
-      <c r="P39" s="1">
+      <c r="P39" s="12">
         <v>0.3045034297643901</v>
       </c>
     </row>
@@ -2272,10 +2271,10 @@
       <c r="F40">
         <v>670</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H40" s="12">
         <v>0.66268656716417906</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I40" s="12">
         <v>0.33731343283582088</v>
       </c>
       <c r="K40">
@@ -2287,10 +2286,10 @@
       <c r="M40">
         <v>49065</v>
       </c>
-      <c r="O40" s="1">
+      <c r="O40" s="12">
         <v>0.80124324875165598</v>
       </c>
-      <c r="P40" s="1">
+      <c r="P40" s="12">
         <v>0.19875675124834402</v>
       </c>
     </row>
@@ -2307,10 +2306,10 @@
       <c r="F41">
         <v>1957</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H41" s="12">
         <v>0.43076136944302501</v>
       </c>
-      <c r="I41" s="1">
+      <c r="I41" s="12">
         <v>0.56923863055697499</v>
       </c>
       <c r="K41">
@@ -2322,10 +2321,10 @@
       <c r="M41">
         <v>146619</v>
       </c>
-      <c r="O41" s="1">
+      <c r="O41" s="12">
         <v>0.53325967303009847</v>
       </c>
-      <c r="P41" s="1">
+      <c r="P41" s="12">
         <v>0.46674032696990159</v>
       </c>
     </row>
@@ -2342,10 +2341,10 @@
       <c r="F42">
         <v>750</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H42" s="12">
         <v>0.68933333333333335</v>
       </c>
-      <c r="I42" s="1">
+      <c r="I42" s="12">
         <v>0.31066666666666665</v>
       </c>
       <c r="K42">
@@ -2357,10 +2356,10 @@
       <c r="M42">
         <v>62431</v>
       </c>
-      <c r="O42" s="1">
+      <c r="O42" s="12">
         <v>0.78307251205330686</v>
       </c>
-      <c r="P42" s="1">
+      <c r="P42" s="12">
         <v>0.21692748794669314</v>
       </c>
     </row>
@@ -2377,10 +2376,10 @@
       <c r="F43">
         <v>837</v>
       </c>
-      <c r="H43" s="1">
+      <c r="H43" s="12">
         <v>0.47909199522102747</v>
       </c>
-      <c r="I43" s="1">
+      <c r="I43" s="12">
         <v>0.52090800477897248</v>
       </c>
       <c r="K43">
@@ -2392,10 +2391,10 @@
       <c r="M43">
         <v>63994</v>
       </c>
-      <c r="O43" s="1">
+      <c r="O43" s="12">
         <v>0.57583523455323937</v>
       </c>
-      <c r="P43" s="1">
+      <c r="P43" s="12">
         <v>0.42416476544676063</v>
       </c>
     </row>
@@ -2404,34 +2403,34 @@
         <v>48</v>
       </c>
       <c r="D44">
-        <v>744</v>
+        <v>749</v>
       </c>
       <c r="E44">
-        <v>1772</v>
+        <v>1767</v>
       </c>
       <c r="F44">
         <v>2516</v>
       </c>
-      <c r="H44" s="1">
-        <v>0.29570747217806043</v>
-      </c>
-      <c r="I44" s="1">
-        <v>0.70429252782193963</v>
+      <c r="H44" s="12">
+        <v>0.29769475357710651</v>
+      </c>
+      <c r="I44" s="12">
+        <v>0.70230524642289349</v>
       </c>
       <c r="K44">
-        <v>68821</v>
+        <v>69145</v>
       </c>
       <c r="L44">
-        <v>116809</v>
+        <v>116485</v>
       </c>
       <c r="M44">
         <v>185630</v>
       </c>
-      <c r="O44" s="1">
-        <v>0.37074287561277813</v>
-      </c>
-      <c r="P44" s="1">
-        <v>0.62925712438722192</v>
+      <c r="O44" s="12">
+        <v>0.37248828314388838</v>
+      </c>
+      <c r="P44" s="12">
+        <v>0.62751171685611162</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
@@ -2439,34 +2438,34 @@
         <v>49</v>
       </c>
       <c r="D45">
-        <v>856</v>
+        <v>860</v>
       </c>
       <c r="E45">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="F45">
         <v>2099</v>
       </c>
-      <c r="H45" s="1">
-        <v>0.40781324440209621</v>
-      </c>
-      <c r="I45" s="1">
-        <v>0.59218675559790379</v>
+      <c r="H45" s="12">
+        <v>0.40971891376846115</v>
+      </c>
+      <c r="I45" s="12">
+        <v>0.59028108623153885</v>
       </c>
       <c r="K45">
-        <v>79236</v>
+        <v>79581</v>
       </c>
       <c r="L45">
-        <v>82138</v>
+        <v>81793</v>
       </c>
       <c r="M45">
         <v>161374</v>
       </c>
-      <c r="O45" s="1">
-        <v>0.49100846480845739</v>
-      </c>
-      <c r="P45" s="1">
-        <v>0.50899153519154261</v>
+      <c r="O45" s="12">
+        <v>0.49314635567067805</v>
+      </c>
+      <c r="P45" s="12">
+        <v>0.5068536443293219</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
@@ -2482,10 +2481,10 @@
       <c r="F46">
         <v>686</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H46" s="12">
         <v>0.43731778425655976</v>
       </c>
-      <c r="I46" s="1">
+      <c r="I46" s="12">
         <v>0.56268221574344024</v>
       </c>
       <c r="K46">
@@ -2497,10 +2496,10 @@
       <c r="M46">
         <v>53982</v>
       </c>
-      <c r="O46" s="1">
+      <c r="O46" s="12">
         <v>0.53034344781593867</v>
       </c>
-      <c r="P46" s="1">
+      <c r="P46" s="12">
         <v>0.46965655218406133</v>
       </c>
     </row>
@@ -2517,10 +2516,10 @@
       <c r="F47">
         <v>823</v>
       </c>
-      <c r="H47" s="1">
+      <c r="H47" s="12">
         <v>0.61239368165249086</v>
       </c>
-      <c r="I47" s="1">
+      <c r="I47" s="12">
         <v>0.38760631834750914</v>
       </c>
       <c r="K47">
@@ -2532,10 +2531,10 @@
       <c r="M47">
         <v>62670</v>
       </c>
-      <c r="O47" s="1">
+      <c r="O47" s="12">
         <v>0.7172171692995053</v>
       </c>
-      <c r="P47" s="1">
+      <c r="P47" s="12">
         <v>0.28278283070049465</v>
       </c>
     </row>
@@ -2544,34 +2543,34 @@
         <v>52</v>
       </c>
       <c r="D48">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="E48">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F48">
         <v>846</v>
       </c>
-      <c r="H48" s="1">
-        <v>0.41371158392434987</v>
-      </c>
-      <c r="I48" s="1">
-        <v>0.58628841607565008</v>
+      <c r="H48" s="12">
+        <v>0.41843971631205673</v>
+      </c>
+      <c r="I48" s="12">
+        <v>0.58156028368794321</v>
       </c>
       <c r="K48">
-        <v>32566</v>
+        <v>32974</v>
       </c>
       <c r="L48">
-        <v>34798</v>
+        <v>34390</v>
       </c>
       <c r="M48">
         <v>67364</v>
       </c>
-      <c r="O48" s="1">
-        <v>0.4834332878095125</v>
-      </c>
-      <c r="P48" s="1">
-        <v>0.51656671219048755</v>
+      <c r="O48" s="12">
+        <v>0.48948993527700257</v>
+      </c>
+      <c r="P48" s="12">
+        <v>0.51051006472299743</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -2587,10 +2586,10 @@
       <c r="F49">
         <v>677</v>
       </c>
-      <c r="H49" s="1">
+      <c r="H49" s="12">
         <v>0.46233382570162479</v>
       </c>
-      <c r="I49" s="1">
+      <c r="I49" s="12">
         <v>0.53766617429837515</v>
       </c>
       <c r="K49">
@@ -2602,10 +2601,10 @@
       <c r="M49">
         <v>54192</v>
       </c>
-      <c r="O49" s="1">
+      <c r="O49" s="12">
         <v>0.55657661647475642</v>
       </c>
-      <c r="P49" s="1">
+      <c r="P49" s="12">
         <v>0.44342338352524358</v>
       </c>
     </row>
@@ -2622,10 +2621,10 @@
       <c r="F50">
         <v>428</v>
       </c>
-      <c r="H50" s="1">
+      <c r="H50" s="12">
         <v>0.68224299065420557</v>
       </c>
-      <c r="I50" s="1">
+      <c r="I50" s="12">
         <v>0.31775700934579437</v>
       </c>
       <c r="K50">
@@ -2637,10 +2636,10 @@
       <c r="M50">
         <v>33241</v>
       </c>
-      <c r="O50" s="1">
+      <c r="O50" s="12">
         <v>0.80388676634276945</v>
       </c>
-      <c r="P50" s="1">
+      <c r="P50" s="12">
         <v>0.19611323365723052</v>
       </c>
     </row>
@@ -2657,10 +2656,10 @@
       <c r="F51">
         <v>1122</v>
       </c>
-      <c r="H51" s="1">
+      <c r="H51" s="12">
         <v>0.6827094474153298</v>
       </c>
-      <c r="I51" s="1">
+      <c r="I51" s="12">
         <v>0.3172905525846702</v>
       </c>
       <c r="K51">
@@ -2672,10 +2671,10 @@
       <c r="M51">
         <v>90258</v>
       </c>
-      <c r="O51" s="1">
+      <c r="O51" s="12">
         <v>0.80257705688138448</v>
       </c>
-      <c r="P51" s="1">
+      <c r="P51" s="12">
         <v>0.19742294311861552</v>
       </c>
     </row>
@@ -2684,34 +2683,34 @@
         <v>56</v>
       </c>
       <c r="D52">
-        <v>2821</v>
+        <v>2831</v>
       </c>
       <c r="E52">
-        <v>1002</v>
+        <v>992</v>
       </c>
       <c r="F52">
         <v>3823</v>
       </c>
-      <c r="H52" s="1">
-        <v>0.73790217106984046</v>
-      </c>
-      <c r="I52" s="1">
-        <v>0.26209782893015954</v>
+      <c r="H52" s="12">
+        <v>0.74051791786555066</v>
+      </c>
+      <c r="I52" s="12">
+        <v>0.2594820821344494</v>
       </c>
       <c r="K52">
-        <v>283013</v>
+        <v>283979</v>
       </c>
       <c r="L52">
-        <v>61331</v>
+        <v>60365</v>
       </c>
       <c r="M52">
         <v>344344</v>
       </c>
-      <c r="O52" s="1">
-        <v>0.82189031898334219</v>
-      </c>
-      <c r="P52" s="1">
-        <v>0.17810968101665775</v>
+      <c r="O52" s="12">
+        <v>0.82469565318402527</v>
+      </c>
+      <c r="P52" s="12">
+        <v>0.17530434681597473</v>
       </c>
     </row>
     <row r="53" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2727,10 +2726,10 @@
       <c r="F53">
         <v>60</v>
       </c>
-      <c r="H53" s="1">
+      <c r="H53" s="12">
         <v>0.8</v>
       </c>
-      <c r="I53" s="1">
+      <c r="I53" s="12">
         <v>0.2</v>
       </c>
       <c r="K53">
@@ -2742,10 +2741,10 @@
       <c r="M53">
         <v>5167</v>
       </c>
-      <c r="O53" s="1">
+      <c r="O53" s="12">
         <v>0.89568414940971552</v>
       </c>
-      <c r="P53" s="1">
+      <c r="P53" s="12">
         <v>0.1043158505902845</v>
       </c>
     </row>
@@ -2756,37 +2755,37 @@
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
       <c r="D54" s="13">
-        <v>25422</v>
+        <v>25692</v>
       </c>
       <c r="E54" s="13">
-        <v>21691</v>
+        <v>21421</v>
       </c>
       <c r="F54" s="13">
         <v>47113</v>
       </c>
       <c r="G54" s="13"/>
       <c r="H54" s="14">
-        <v>0.53959628977140073</v>
+        <v>0.54532719207012925</v>
       </c>
       <c r="I54" s="14">
-        <v>0.46040371022859933</v>
+        <v>0.45467280792987075</v>
       </c>
       <c r="J54" s="13"/>
       <c r="K54" s="13">
-        <v>2388136</v>
+        <v>2412713</v>
       </c>
       <c r="L54" s="13">
-        <v>1352578</v>
+        <v>1328001</v>
       </c>
       <c r="M54" s="13">
         <v>3740714</v>
       </c>
       <c r="N54" s="13"/>
       <c r="O54" s="14">
-        <v>0.63841715779393993</v>
+        <v>0.6449872938695661</v>
       </c>
       <c r="P54" s="14">
-        <v>0.36158284220606013</v>
+        <v>0.3550127061304339</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -2805,10 +2804,10 @@
       <c r="F55">
         <v>285</v>
       </c>
-      <c r="H55" s="1">
+      <c r="H55" s="12">
         <v>0.72280701754385968</v>
       </c>
-      <c r="I55" s="1">
+      <c r="I55" s="12">
         <v>0.27719298245614032</v>
       </c>
       <c r="K55">
@@ -2820,10 +2819,10 @@
       <c r="M55">
         <v>22926</v>
       </c>
-      <c r="O55" s="1">
+      <c r="O55" s="12">
         <v>0.81261449882229786</v>
       </c>
-      <c r="P55" s="1">
+      <c r="P55" s="12">
         <v>0.18738550117770217</v>
       </c>
     </row>
@@ -2840,10 +2839,10 @@
       <c r="F56">
         <v>81</v>
       </c>
-      <c r="H56" s="1">
+      <c r="H56" s="12">
         <v>0.8271604938271605</v>
       </c>
-      <c r="I56" s="1">
+      <c r="I56" s="12">
         <v>0.1728395061728395</v>
       </c>
       <c r="K56">
@@ -2855,10 +2854,10 @@
       <c r="M56">
         <v>6910</v>
       </c>
-      <c r="O56" s="1">
+      <c r="O56" s="12">
         <v>0.87829232995658468</v>
       </c>
-      <c r="P56" s="1">
+      <c r="P56" s="12">
         <v>0.12170767004341534</v>
       </c>
     </row>
@@ -2875,10 +2874,10 @@
       <c r="F57">
         <v>242</v>
       </c>
-      <c r="H57" s="1">
+      <c r="H57" s="12">
         <v>0.47933884297520662</v>
       </c>
-      <c r="I57" s="1">
+      <c r="I57" s="12">
         <v>0.52066115702479343</v>
       </c>
       <c r="K57">
@@ -2890,10 +2889,10 @@
       <c r="M57">
         <v>18986</v>
       </c>
-      <c r="O57" s="1">
+      <c r="O57" s="12">
         <v>0.5708416728115453</v>
       </c>
-      <c r="P57" s="1">
+      <c r="P57" s="12">
         <v>0.42915832718845465</v>
       </c>
     </row>
@@ -2910,10 +2909,10 @@
       <c r="F58">
         <v>68</v>
       </c>
-      <c r="H58" s="1">
+      <c r="H58" s="12">
         <v>0.76470588235294112</v>
       </c>
-      <c r="I58" s="1">
+      <c r="I58" s="12">
         <v>0.23529411764705882</v>
       </c>
       <c r="K58">
@@ -2925,10 +2924,10 @@
       <c r="M58">
         <v>5417</v>
       </c>
-      <c r="O58" s="1">
+      <c r="O58" s="12">
         <v>0.80450433819457268</v>
       </c>
-      <c r="P58" s="1">
+      <c r="P58" s="12">
         <v>0.19549566180542735</v>
       </c>
     </row>
@@ -2945,10 +2944,10 @@
       <c r="F59">
         <v>163</v>
       </c>
-      <c r="H59" s="1">
+      <c r="H59" s="12">
         <v>0.63190184049079756</v>
       </c>
-      <c r="I59" s="1">
+      <c r="I59" s="12">
         <v>0.36809815950920244</v>
       </c>
       <c r="K59">
@@ -2960,10 +2959,10 @@
       <c r="M59">
         <v>13710</v>
       </c>
-      <c r="O59" s="1">
+      <c r="O59" s="12">
         <v>0.70547045951859955</v>
       </c>
-      <c r="P59" s="1">
+      <c r="P59" s="12">
         <v>0.29452954048140045</v>
       </c>
     </row>
@@ -2980,10 +2979,10 @@
       <c r="F60">
         <v>104</v>
       </c>
-      <c r="H60" s="1">
+      <c r="H60" s="12">
         <v>0.69230769230769229</v>
       </c>
-      <c r="I60" s="1">
+      <c r="I60" s="12">
         <v>0.30769230769230771</v>
       </c>
       <c r="K60">
@@ -2995,10 +2994,10 @@
       <c r="M60">
         <v>7610</v>
       </c>
-      <c r="O60" s="1">
+      <c r="O60" s="12">
         <v>0.83968462549277267</v>
       </c>
-      <c r="P60" s="1">
+      <c r="P60" s="12">
         <v>0.16031537450722733</v>
       </c>
     </row>
@@ -3058,10 +3057,10 @@
       <c r="F62">
         <v>37</v>
       </c>
-      <c r="H62" s="1">
+      <c r="H62" s="12">
         <v>0.45945945945945948</v>
       </c>
-      <c r="I62" s="1">
+      <c r="I62" s="12">
         <v>0.54054054054054057</v>
       </c>
       <c r="K62">
@@ -3073,10 +3072,10 @@
       <c r="M62">
         <v>3033</v>
       </c>
-      <c r="O62" s="1">
+      <c r="O62" s="12">
         <v>0.63303659742828877</v>
       </c>
-      <c r="P62" s="1">
+      <c r="P62" s="12">
         <v>0.36696340257171117</v>
       </c>
     </row>
@@ -3093,10 +3092,10 @@
       <c r="F63">
         <v>59</v>
       </c>
-      <c r="H63" s="1">
+      <c r="H63" s="12">
         <v>0.33898305084745761</v>
       </c>
-      <c r="I63" s="1">
+      <c r="I63" s="12">
         <v>0.66101694915254239</v>
       </c>
       <c r="K63">
@@ -3108,10 +3107,10 @@
       <c r="M63">
         <v>4163</v>
       </c>
-      <c r="O63" s="1">
+      <c r="O63" s="12">
         <v>0.38770117703579149</v>
       </c>
-      <c r="P63" s="1">
+      <c r="P63" s="12">
         <v>0.61229882296420846</v>
       </c>
     </row>
@@ -3128,10 +3127,10 @@
       <c r="F64">
         <v>88</v>
       </c>
-      <c r="H64" s="1">
+      <c r="H64" s="12">
         <v>0.34090909090909088</v>
       </c>
-      <c r="I64" s="1">
+      <c r="I64" s="12">
         <v>0.65909090909090906</v>
       </c>
       <c r="K64">
@@ -3143,10 +3142,10 @@
       <c r="M64">
         <v>6243</v>
       </c>
-      <c r="O64" s="1">
+      <c r="O64" s="12">
         <v>0.43200384430562228</v>
       </c>
-      <c r="P64" s="1">
+      <c r="P64" s="12">
         <v>0.56799615569437767</v>
       </c>
     </row>
@@ -3163,10 +3162,10 @@
       <c r="F65">
         <v>220</v>
       </c>
-      <c r="H65" s="1">
+      <c r="H65" s="12">
         <v>0.32272727272727275</v>
       </c>
-      <c r="I65" s="1">
+      <c r="I65" s="12">
         <v>0.67727272727272725</v>
       </c>
       <c r="K65">
@@ -3178,10 +3177,10 @@
       <c r="M65">
         <v>15438</v>
       </c>
-      <c r="O65" s="1">
+      <c r="O65" s="12">
         <v>0.41423759554346418</v>
       </c>
-      <c r="P65" s="1">
+      <c r="P65" s="12">
         <v>0.58576240445653582</v>
       </c>
     </row>
@@ -3198,10 +3197,10 @@
       <c r="F66">
         <v>115</v>
       </c>
-      <c r="H66" s="1">
+      <c r="H66" s="12">
         <v>0.5043478260869565</v>
       </c>
-      <c r="I66" s="1">
+      <c r="I66" s="12">
         <v>0.4956521739130435</v>
       </c>
       <c r="K66">
@@ -3213,10 +3212,10 @@
       <c r="M66">
         <v>7768</v>
       </c>
-      <c r="O66" s="1">
+      <c r="O66" s="12">
         <v>0.52677651905252321</v>
       </c>
-      <c r="P66" s="1">
+      <c r="P66" s="12">
         <v>0.47322348094747685</v>
       </c>
     </row>
@@ -3233,10 +3232,10 @@
       <c r="F67">
         <v>271</v>
       </c>
-      <c r="H67" s="1">
+      <c r="H67" s="12">
         <v>0.36531365313653136</v>
       </c>
-      <c r="I67" s="1">
+      <c r="I67" s="12">
         <v>0.63468634686346859</v>
       </c>
       <c r="K67">
@@ -3248,10 +3247,10 @@
       <c r="M67">
         <v>19720</v>
       </c>
-      <c r="O67" s="1">
+      <c r="O67" s="12">
         <v>0.43884381338742395</v>
       </c>
-      <c r="P67" s="1">
+      <c r="P67" s="12">
         <v>0.56115618661257605</v>
       </c>
     </row>
@@ -3268,10 +3267,10 @@
       <c r="F68">
         <v>100</v>
       </c>
-      <c r="H68" s="1">
+      <c r="H68" s="12">
         <v>0.53</v>
       </c>
-      <c r="I68" s="1">
+      <c r="I68" s="12">
         <v>0.47</v>
       </c>
       <c r="K68">
@@ -3283,10 +3282,10 @@
       <c r="M68">
         <v>7632</v>
       </c>
-      <c r="O68" s="1">
+      <c r="O68" s="12">
         <v>0.62866876310272535</v>
       </c>
-      <c r="P68" s="1">
+      <c r="P68" s="12">
         <v>0.37133123689727465</v>
       </c>
     </row>
@@ -3303,10 +3302,10 @@
       <c r="F69">
         <v>119</v>
       </c>
-      <c r="H69" s="1">
+      <c r="H69" s="12">
         <v>0.45378151260504201</v>
       </c>
-      <c r="I69" s="1">
+      <c r="I69" s="12">
         <v>0.54621848739495793</v>
       </c>
       <c r="K69">
@@ -3318,10 +3317,10 @@
       <c r="M69">
         <v>8660</v>
       </c>
-      <c r="O69" s="1">
+      <c r="O69" s="12">
         <v>0.56200923787528867</v>
       </c>
-      <c r="P69" s="1">
+      <c r="P69" s="12">
         <v>0.43799076212471133</v>
       </c>
     </row>
@@ -3338,10 +3337,10 @@
       <c r="F70">
         <v>46</v>
       </c>
-      <c r="H70" s="1">
+      <c r="H70" s="12">
         <v>0.13043478260869565</v>
       </c>
-      <c r="I70" s="1">
+      <c r="I70" s="12">
         <v>0.86956521739130432</v>
       </c>
       <c r="K70">
@@ -3353,10 +3352,10 @@
       <c r="M70">
         <v>2926</v>
       </c>
-      <c r="O70" s="1">
+      <c r="O70" s="12">
         <v>0.24504442925495556</v>
       </c>
-      <c r="P70" s="1">
+      <c r="P70" s="12">
         <v>0.75495557074504438</v>
       </c>
     </row>
@@ -3373,10 +3372,10 @@
       <c r="F71">
         <v>78</v>
       </c>
-      <c r="H71" s="1">
+      <c r="H71" s="12">
         <v>0.46153846153846156</v>
       </c>
-      <c r="I71" s="1">
+      <c r="I71" s="12">
         <v>0.53846153846153844</v>
       </c>
       <c r="K71">
@@ -3388,10 +3387,10 @@
       <c r="M71">
         <v>5888</v>
       </c>
-      <c r="O71" s="1">
+      <c r="O71" s="12">
         <v>0.53277853260869568</v>
       </c>
-      <c r="P71" s="1">
+      <c r="P71" s="12">
         <v>0.46722146739130432</v>
       </c>
     </row>
@@ -3408,10 +3407,10 @@
       <c r="F72">
         <v>66</v>
       </c>
-      <c r="H72" s="1">
+      <c r="H72" s="12">
         <v>0.51515151515151514</v>
       </c>
-      <c r="I72" s="1">
+      <c r="I72" s="12">
         <v>0.48484848484848486</v>
       </c>
       <c r="K72">
@@ -3423,10 +3422,10 @@
       <c r="M72">
         <v>5681</v>
       </c>
-      <c r="O72" s="1">
+      <c r="O72" s="12">
         <v>0.56891392360499915</v>
       </c>
-      <c r="P72" s="1">
+      <c r="P72" s="12">
         <v>0.43108607639500091</v>
       </c>
     </row>
@@ -3443,10 +3442,10 @@
       <c r="F73">
         <v>31</v>
       </c>
-      <c r="H73" s="1">
+      <c r="H73" s="12">
         <v>0.32258064516129031</v>
       </c>
-      <c r="I73" s="1">
+      <c r="I73" s="12">
         <v>0.67741935483870963</v>
       </c>
       <c r="K73">
@@ -3458,10 +3457,10 @@
       <c r="M73">
         <v>2447</v>
       </c>
-      <c r="O73" s="1">
+      <c r="O73" s="12">
         <v>0.4765018389865141</v>
       </c>
-      <c r="P73" s="1">
+      <c r="P73" s="12">
         <v>0.5234981610134859</v>
       </c>
     </row>
@@ -3478,10 +3477,10 @@
       <c r="F74">
         <v>79</v>
       </c>
-      <c r="H74" s="1">
+      <c r="H74" s="12">
         <v>0.25316455696202533</v>
       </c>
-      <c r="I74" s="1">
+      <c r="I74" s="12">
         <v>0.74683544303797467</v>
       </c>
       <c r="K74">
@@ -3493,10 +3492,10 @@
       <c r="M74">
         <v>5888</v>
       </c>
-      <c r="O74" s="1">
+      <c r="O74" s="12">
         <v>0.28923233695652173</v>
       </c>
-      <c r="P74" s="1">
+      <c r="P74" s="12">
         <v>0.71076766304347827</v>
       </c>
     </row>
@@ -3513,10 +3512,10 @@
       <c r="F75">
         <v>33</v>
       </c>
-      <c r="H75" s="1">
+      <c r="H75" s="12">
         <v>0.24242424242424243</v>
       </c>
-      <c r="I75" s="1">
+      <c r="I75" s="12">
         <v>0.75757575757575757</v>
       </c>
       <c r="K75">
@@ -3528,10 +3527,10 @@
       <c r="M75">
         <v>2443</v>
       </c>
-      <c r="O75" s="1">
+      <c r="O75" s="12">
         <v>0.17560376586164553</v>
       </c>
-      <c r="P75" s="1">
+      <c r="P75" s="12">
         <v>0.8243962341383545</v>
       </c>
     </row>
@@ -3548,10 +3547,10 @@
       <c r="F76">
         <v>52</v>
       </c>
-      <c r="H76" s="1">
+      <c r="H76" s="12">
         <v>0.48076923076923078</v>
       </c>
-      <c r="I76" s="1">
+      <c r="I76" s="12">
         <v>0.51923076923076927</v>
       </c>
       <c r="K76">
@@ -3563,10 +3562,10 @@
       <c r="M76">
         <v>4042</v>
       </c>
-      <c r="O76" s="1">
+      <c r="O76" s="12">
         <v>0.59698169223156849</v>
       </c>
-      <c r="P76" s="1">
+      <c r="P76" s="12">
         <v>0.40301830776843145</v>
       </c>
     </row>
@@ -3583,10 +3582,10 @@
       <c r="F77">
         <v>93</v>
       </c>
-      <c r="H77" s="1">
+      <c r="H77" s="12">
         <v>0.30107526881720431</v>
       </c>
-      <c r="I77" s="1">
+      <c r="I77" s="12">
         <v>0.69892473118279574</v>
       </c>
       <c r="K77">
@@ -3598,10 +3597,10 @@
       <c r="M77">
         <v>6684</v>
       </c>
-      <c r="O77" s="1">
+      <c r="O77" s="12">
         <v>0.31403351286654696</v>
       </c>
-      <c r="P77" s="1">
+      <c r="P77" s="12">
         <v>0.68596648713345298</v>
       </c>
     </row>
@@ -3618,10 +3617,10 @@
       <c r="F78">
         <v>65</v>
       </c>
-      <c r="H78" s="1">
+      <c r="H78" s="12">
         <v>0.26153846153846155</v>
       </c>
-      <c r="I78" s="1">
+      <c r="I78" s="12">
         <v>0.7384615384615385</v>
       </c>
       <c r="K78">
@@ -3633,10 +3632,10 @@
       <c r="M78">
         <v>5234</v>
       </c>
-      <c r="O78" s="1">
+      <c r="O78" s="12">
         <v>0.32976690867405428</v>
       </c>
-      <c r="P78" s="1">
+      <c r="P78" s="12">
         <v>0.67023309132594577</v>
       </c>
     </row>
@@ -3653,10 +3652,10 @@
       <c r="F79">
         <v>15</v>
       </c>
-      <c r="H79" s="1">
+      <c r="H79" s="12">
         <v>0.73333333333333328</v>
       </c>
-      <c r="I79" s="1">
+      <c r="I79" s="12">
         <v>0.26666666666666666</v>
       </c>
       <c r="K79">
@@ -3668,10 +3667,10 @@
       <c r="M79">
         <v>1200</v>
       </c>
-      <c r="O79" s="1">
+      <c r="O79" s="12">
         <v>0.84666666666666668</v>
       </c>
-      <c r="P79" s="1">
+      <c r="P79" s="12">
         <v>0.15333333333333332</v>
       </c>
     </row>
@@ -3688,10 +3687,10 @@
       <c r="F80">
         <v>37</v>
       </c>
-      <c r="H80" s="1">
+      <c r="H80" s="12">
         <v>0.27027027027027029</v>
       </c>
-      <c r="I80" s="1">
+      <c r="I80" s="12">
         <v>0.72972972972972971</v>
       </c>
       <c r="K80">
@@ -3703,10 +3702,10 @@
       <c r="M80">
         <v>2475</v>
       </c>
-      <c r="O80" s="1">
+      <c r="O80" s="12">
         <v>0.34989898989898988</v>
       </c>
-      <c r="P80" s="1">
+      <c r="P80" s="12">
         <v>0.65010101010101007</v>
       </c>
     </row>
@@ -3723,10 +3722,10 @@
       <c r="F81">
         <v>31</v>
       </c>
-      <c r="H81" s="1">
+      <c r="H81" s="12">
         <v>0.29032258064516131</v>
       </c>
-      <c r="I81" s="1">
+      <c r="I81" s="12">
         <v>0.70967741935483875</v>
       </c>
       <c r="K81">
@@ -3738,10 +3737,10 @@
       <c r="M81">
         <v>1846</v>
       </c>
-      <c r="O81" s="1">
+      <c r="O81" s="12">
         <v>0.53033586132177679</v>
       </c>
-      <c r="P81" s="1">
+      <c r="P81" s="12">
         <v>0.46966413867822321</v>
       </c>
     </row>
@@ -3758,10 +3757,10 @@
       <c r="F82">
         <v>39</v>
       </c>
-      <c r="H82" s="1">
+      <c r="H82" s="12">
         <v>0.66666666666666663</v>
       </c>
-      <c r="I82" s="1">
+      <c r="I82" s="12">
         <v>0.33333333333333331</v>
       </c>
       <c r="K82">
@@ -3773,10 +3772,10 @@
       <c r="M82">
         <v>3281</v>
       </c>
-      <c r="O82" s="1">
+      <c r="O82" s="12">
         <v>0.73940871685461751</v>
       </c>
-      <c r="P82" s="1">
+      <c r="P82" s="12">
         <v>0.26059128314538249</v>
       </c>
     </row>
@@ -3793,10 +3792,10 @@
       <c r="F83">
         <v>130</v>
       </c>
-      <c r="H83" s="1">
+      <c r="H83" s="12">
         <v>0.23846153846153847</v>
       </c>
-      <c r="I83" s="1">
+      <c r="I83" s="12">
         <v>0.7615384615384615</v>
       </c>
       <c r="K83">
@@ -3808,10 +3807,10 @@
       <c r="M83">
         <v>9172</v>
       </c>
-      <c r="O83" s="1">
+      <c r="O83" s="12">
         <v>0.29164849542084603</v>
       </c>
-      <c r="P83" s="1">
+      <c r="P83" s="12">
         <v>0.70835150457915397</v>
       </c>
     </row>
@@ -3828,10 +3827,10 @@
       <c r="F84">
         <v>106</v>
       </c>
-      <c r="H84" s="1">
+      <c r="H84" s="12">
         <v>0.55660377358490565</v>
       </c>
-      <c r="I84" s="1">
+      <c r="I84" s="12">
         <v>0.44339622641509435</v>
       </c>
       <c r="K84">
@@ -3843,10 +3842,10 @@
       <c r="M84">
         <v>8309</v>
       </c>
-      <c r="O84" s="1">
+      <c r="O84" s="12">
         <v>0.66891322662173547</v>
       </c>
-      <c r="P84" s="1">
+      <c r="P84" s="12">
         <v>0.33108677337826453</v>
       </c>
     </row>
@@ -3863,10 +3862,10 @@
       <c r="F85">
         <v>50</v>
       </c>
-      <c r="H85" s="1">
+      <c r="H85" s="12">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I85" s="1">
+      <c r="I85" s="12">
         <v>0.44</v>
       </c>
       <c r="K85">
@@ -3878,10 +3877,10 @@
       <c r="M85">
         <v>4660</v>
       </c>
-      <c r="O85" s="1">
+      <c r="O85" s="12">
         <v>0.65901287553648069</v>
       </c>
-      <c r="P85" s="1">
+      <c r="P85" s="12">
         <v>0.34098712446351931</v>
       </c>
     </row>
@@ -3898,10 +3897,10 @@
       <c r="F86">
         <v>76</v>
       </c>
-      <c r="H86" s="1">
+      <c r="H86" s="12">
         <v>0.34210526315789475</v>
       </c>
-      <c r="I86" s="1">
+      <c r="I86" s="12">
         <v>0.65789473684210531</v>
       </c>
       <c r="K86">
@@ -3913,10 +3912,10 @@
       <c r="M86">
         <v>6435</v>
       </c>
-      <c r="O86" s="1">
+      <c r="O86" s="12">
         <v>0.43729603729603728</v>
       </c>
-      <c r="P86" s="1">
+      <c r="P86" s="12">
         <v>0.56270396270396272</v>
       </c>
     </row>
@@ -3933,10 +3932,10 @@
       <c r="F87">
         <v>113</v>
       </c>
-      <c r="H87" s="1">
+      <c r="H87" s="12">
         <v>0.34513274336283184</v>
       </c>
-      <c r="I87" s="1">
+      <c r="I87" s="12">
         <v>0.65486725663716816</v>
       </c>
       <c r="K87">
@@ -3948,10 +3947,10 @@
       <c r="M87">
         <v>8329</v>
       </c>
-      <c r="O87" s="1">
+      <c r="O87" s="12">
         <v>0.42442069876335692</v>
       </c>
-      <c r="P87" s="1">
+      <c r="P87" s="12">
         <v>0.57557930123664303</v>
       </c>
     </row>
@@ -4011,10 +4010,10 @@
       <c r="F89">
         <v>155</v>
       </c>
-      <c r="H89" s="1">
+      <c r="H89" s="12">
         <v>0.5741935483870968</v>
       </c>
-      <c r="I89" s="1">
+      <c r="I89" s="12">
         <v>0.4258064516129032</v>
       </c>
       <c r="K89">
@@ -4026,10 +4025,10 @@
       <c r="M89">
         <v>12476</v>
       </c>
-      <c r="O89" s="1">
+      <c r="O89" s="12">
         <v>0.69501442770118627</v>
       </c>
-      <c r="P89" s="1">
+      <c r="P89" s="12">
         <v>0.30498557229881373</v>
       </c>
     </row>
@@ -4089,10 +4088,10 @@
       <c r="F91">
         <v>481</v>
       </c>
-      <c r="H91" s="1">
+      <c r="H91" s="12">
         <v>0.64033264033264037</v>
       </c>
-      <c r="I91" s="1">
+      <c r="I91" s="12">
         <v>0.35966735966735969</v>
       </c>
       <c r="K91">
@@ -4104,10 +4103,10 @@
       <c r="M91">
         <v>38674</v>
       </c>
-      <c r="O91" s="1">
+      <c r="O91" s="12">
         <v>0.73811863267311373</v>
       </c>
-      <c r="P91" s="1">
+      <c r="P91" s="12">
         <v>0.26188136732688627</v>
       </c>
     </row>
@@ -4124,10 +4123,10 @@
       <c r="F92">
         <v>460</v>
       </c>
-      <c r="H92" s="1">
+      <c r="H92" s="12">
         <v>0.81739130434782614</v>
       </c>
-      <c r="I92" s="1">
+      <c r="I92" s="12">
         <v>0.18260869565217391</v>
       </c>
       <c r="K92">
@@ -4139,10 +4138,10 @@
       <c r="M92">
         <v>40489</v>
       </c>
-      <c r="O92" s="1">
+      <c r="O92" s="12">
         <v>0.86969300303786212</v>
       </c>
-      <c r="P92" s="1">
+      <c r="P92" s="12">
         <v>0.13030699696213788</v>
       </c>
     </row>
@@ -4159,10 +4158,10 @@
       <c r="F93">
         <v>903</v>
       </c>
-      <c r="H93" s="1">
+      <c r="H93" s="12">
         <v>0.64784053156146182</v>
       </c>
-      <c r="I93" s="1">
+      <c r="I93" s="12">
         <v>0.35215946843853818</v>
       </c>
       <c r="K93">
@@ -4174,10 +4173,10 @@
       <c r="M93">
         <v>75481</v>
       </c>
-      <c r="O93" s="1">
+      <c r="O93" s="12">
         <v>0.73846398431393334</v>
       </c>
-      <c r="P93" s="1">
+      <c r="P93" s="12">
         <v>0.26153601568606671</v>
       </c>
     </row>
@@ -4186,34 +4185,34 @@
         <v>101</v>
       </c>
       <c r="D94">
-        <v>446</v>
+        <v>458</v>
       </c>
       <c r="E94">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="F94">
         <v>669</v>
       </c>
-      <c r="H94" s="1">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="I94" s="1">
-        <v>0.33333333333333331</v>
+      <c r="H94" s="12">
+        <v>0.68460388639760839</v>
+      </c>
+      <c r="I94" s="12">
+        <v>0.31539611360239161</v>
       </c>
       <c r="K94">
-        <v>42259</v>
+        <v>43400</v>
       </c>
       <c r="L94">
-        <v>15408</v>
+        <v>14267</v>
       </c>
       <c r="M94">
         <v>57667</v>
       </c>
-      <c r="O94" s="1">
-        <v>0.73281079300119656</v>
-      </c>
-      <c r="P94" s="1">
-        <v>0.2671892069988035</v>
+      <c r="O94" s="12">
+        <v>0.75259680579881039</v>
+      </c>
+      <c r="P94" s="12">
+        <v>0.24740319420118959</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
@@ -4229,10 +4228,10 @@
       <c r="F95">
         <v>99</v>
       </c>
-      <c r="H95" s="1">
+      <c r="H95" s="12">
         <v>0.79797979797979801</v>
       </c>
-      <c r="I95" s="1">
+      <c r="I95" s="12">
         <v>0.20202020202020202</v>
       </c>
       <c r="K95">
@@ -4244,10 +4243,10 @@
       <c r="M95">
         <v>8375</v>
       </c>
-      <c r="O95" s="1">
+      <c r="O95" s="12">
         <v>0.87904477611940302</v>
       </c>
-      <c r="P95" s="1">
+      <c r="P95" s="12">
         <v>0.12095522388059701</v>
       </c>
     </row>
@@ -4264,10 +4263,10 @@
       <c r="F96">
         <v>148</v>
       </c>
-      <c r="H96" s="1">
+      <c r="H96" s="12">
         <v>0.80405405405405406</v>
       </c>
-      <c r="I96" s="1">
+      <c r="I96" s="12">
         <v>0.19594594594594594</v>
       </c>
       <c r="K96">
@@ -4279,10 +4278,10 @@
       <c r="M96">
         <v>12049</v>
       </c>
-      <c r="O96" s="1">
+      <c r="O96" s="12">
         <v>0.88804050128641376</v>
       </c>
-      <c r="P96" s="1">
+      <c r="P96" s="12">
         <v>0.11195949871358619</v>
       </c>
     </row>
@@ -4299,10 +4298,10 @@
       <c r="F97">
         <v>97</v>
       </c>
-      <c r="H97" s="1">
+      <c r="H97" s="12">
         <v>0.87628865979381443</v>
       </c>
-      <c r="I97" s="1">
+      <c r="I97" s="12">
         <v>0.12371134020618557</v>
       </c>
       <c r="K97">
@@ -4314,10 +4313,10 @@
       <c r="M97">
         <v>8171</v>
       </c>
-      <c r="O97" s="1">
+      <c r="O97" s="12">
         <v>0.94994492718149548</v>
       </c>
-      <c r="P97" s="1">
+      <c r="P97" s="12">
         <v>5.0055072818504465E-2</v>
       </c>
     </row>
@@ -4334,10 +4333,10 @@
       <c r="F98">
         <v>117</v>
       </c>
-      <c r="H98" s="1">
+      <c r="H98" s="12">
         <v>0.83760683760683763</v>
       </c>
-      <c r="I98" s="1">
+      <c r="I98" s="12">
         <v>0.1623931623931624</v>
       </c>
       <c r="K98">
@@ -4349,10 +4348,10 @@
       <c r="M98">
         <v>10528</v>
       </c>
-      <c r="O98" s="1">
+      <c r="O98" s="12">
         <v>0.93199088145896658</v>
       </c>
-      <c r="P98" s="1">
+      <c r="P98" s="12">
         <v>6.8009118541033434E-2</v>
       </c>
     </row>
@@ -4369,10 +4368,10 @@
       <c r="F99">
         <v>70</v>
       </c>
-      <c r="H99" s="1">
+      <c r="H99" s="12">
         <v>0.97142857142857142</v>
       </c>
-      <c r="I99" s="1">
+      <c r="I99" s="12">
         <v>2.8571428571428571E-2</v>
       </c>
       <c r="K99">
@@ -4384,10 +4383,10 @@
       <c r="M99">
         <v>6020</v>
       </c>
-      <c r="O99" s="1">
+      <c r="O99" s="12">
         <v>0.9963455149501661</v>
       </c>
-      <c r="P99" s="1">
+      <c r="P99" s="12">
         <v>3.6544850498338869E-3</v>
       </c>
     </row>
@@ -4404,10 +4403,10 @@
       <c r="F100">
         <v>365</v>
       </c>
-      <c r="H100" s="1">
+      <c r="H100" s="12">
         <v>0.71780821917808224</v>
       </c>
-      <c r="I100" s="1">
+      <c r="I100" s="12">
         <v>0.28219178082191781</v>
       </c>
       <c r="K100">
@@ -4419,10 +4418,10 @@
       <c r="M100">
         <v>26835</v>
       </c>
-      <c r="O100" s="1">
+      <c r="O100" s="12">
         <v>0.81464505310229174</v>
       </c>
-      <c r="P100" s="1">
+      <c r="P100" s="12">
         <v>0.18535494689770821</v>
       </c>
     </row>
@@ -4431,34 +4430,34 @@
         <v>108</v>
       </c>
       <c r="D101">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E101">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F101">
         <v>244</v>
       </c>
-      <c r="H101" s="1">
-        <v>0.59426229508196726</v>
-      </c>
-      <c r="I101" s="1">
-        <v>0.40573770491803279</v>
+      <c r="H101" s="12">
+        <v>0.61065573770491799</v>
+      </c>
+      <c r="I101" s="12">
+        <v>0.38934426229508196</v>
       </c>
       <c r="K101">
-        <v>13214</v>
+        <v>13682</v>
       </c>
       <c r="L101">
-        <v>6143</v>
+        <v>5675</v>
       </c>
       <c r="M101">
         <v>19357</v>
       </c>
-      <c r="O101" s="1">
-        <v>0.68264710440667464</v>
-      </c>
-      <c r="P101" s="1">
-        <v>0.31735289559332541</v>
+      <c r="O101" s="12">
+        <v>0.7068244046081521</v>
+      </c>
+      <c r="P101" s="12">
+        <v>0.2931755953918479</v>
       </c>
     </row>
     <row r="102" spans="2:16" x14ac:dyDescent="0.25">
@@ -4474,10 +4473,10 @@
       <c r="F102">
         <v>175</v>
       </c>
-      <c r="H102" s="1">
+      <c r="H102" s="12">
         <v>0.81714285714285717</v>
       </c>
-      <c r="I102" s="1">
+      <c r="I102" s="12">
         <v>0.18285714285714286</v>
       </c>
       <c r="K102">
@@ -4489,10 +4488,10 @@
       <c r="M102">
         <v>13756</v>
       </c>
-      <c r="O102" s="1">
+      <c r="O102" s="12">
         <v>0.88325094504216339</v>
       </c>
-      <c r="P102" s="1">
+      <c r="P102" s="12">
         <v>0.11674905495783658</v>
       </c>
     </row>
@@ -4509,10 +4508,10 @@
       <c r="F103">
         <v>381</v>
       </c>
-      <c r="H103" s="1">
+      <c r="H103" s="12">
         <v>0.66141732283464572</v>
       </c>
-      <c r="I103" s="1">
+      <c r="I103" s="12">
         <v>0.33858267716535434</v>
       </c>
       <c r="K103">
@@ -4524,10 +4523,10 @@
       <c r="M103">
         <v>33844</v>
       </c>
-      <c r="O103" s="1">
+      <c r="O103" s="12">
         <v>0.75345703817515663</v>
       </c>
-      <c r="P103" s="1">
+      <c r="P103" s="12">
         <v>0.24654296182484339</v>
       </c>
     </row>
@@ -4536,34 +4535,34 @@
         <v>111</v>
       </c>
       <c r="D104">
-        <v>613</v>
+        <v>617</v>
       </c>
       <c r="E104">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F104">
         <v>893</v>
       </c>
-      <c r="H104" s="1">
-        <v>0.6864501679731243</v>
-      </c>
-      <c r="I104" s="1">
-        <v>0.3135498320268757</v>
+      <c r="H104" s="12">
+        <v>0.69092945128779393</v>
+      </c>
+      <c r="I104" s="12">
+        <v>0.30907054871220607</v>
       </c>
       <c r="K104">
-        <v>54168</v>
+        <v>54430</v>
       </c>
       <c r="L104">
-        <v>15161</v>
+        <v>14899</v>
       </c>
       <c r="M104">
         <v>69329</v>
       </c>
-      <c r="O104" s="1">
-        <v>0.78131806314817753</v>
-      </c>
-      <c r="P104" s="1">
-        <v>0.21868193685182247</v>
+      <c r="O104" s="12">
+        <v>0.78509714549467036</v>
+      </c>
+      <c r="P104" s="12">
+        <v>0.21490285450532967</v>
       </c>
     </row>
     <row r="105" spans="2:16" x14ac:dyDescent="0.25">
@@ -4579,10 +4578,10 @@
       <c r="F105">
         <v>145</v>
       </c>
-      <c r="H105" s="1">
+      <c r="H105" s="12">
         <v>0.77241379310344827</v>
       </c>
-      <c r="I105" s="1">
+      <c r="I105" s="12">
         <v>0.22758620689655173</v>
       </c>
       <c r="K105">
@@ -4594,10 +4593,10 @@
       <c r="M105">
         <v>12605</v>
       </c>
-      <c r="O105" s="1">
+      <c r="O105" s="12">
         <v>0.85085283617612062</v>
       </c>
-      <c r="P105" s="1">
+      <c r="P105" s="12">
         <v>0.14914716382387941</v>
       </c>
     </row>
@@ -4614,10 +4613,10 @@
       <c r="F106">
         <v>48</v>
       </c>
-      <c r="H106" s="1">
+      <c r="H106" s="12">
         <v>0.70833333333333337</v>
       </c>
-      <c r="I106" s="1">
+      <c r="I106" s="12">
         <v>0.29166666666666669</v>
       </c>
       <c r="K106">
@@ -4629,10 +4628,10 @@
       <c r="M106">
         <v>4569</v>
       </c>
-      <c r="O106" s="1">
+      <c r="O106" s="12">
         <v>0.72050776975268116</v>
       </c>
-      <c r="P106" s="1">
+      <c r="P106" s="12">
         <v>0.2794922302473189</v>
       </c>
     </row>
@@ -4649,10 +4648,10 @@
       <c r="F107">
         <v>296</v>
       </c>
-      <c r="H107" s="1">
+      <c r="H107" s="12">
         <v>0.73310810810810811</v>
       </c>
-      <c r="I107" s="1">
+      <c r="I107" s="12">
         <v>0.26689189189189189</v>
       </c>
       <c r="K107">
@@ -4664,10 +4663,10 @@
       <c r="M107">
         <v>23980</v>
       </c>
-      <c r="O107" s="1">
+      <c r="O107" s="12">
         <v>0.8055879899916597</v>
       </c>
-      <c r="P107" s="1">
+      <c r="P107" s="12">
         <v>0.1944120100083403</v>
       </c>
     </row>
@@ -4684,10 +4683,10 @@
       <c r="F108">
         <v>537</v>
       </c>
-      <c r="H108" s="1">
+      <c r="H108" s="12">
         <v>0.70577281191806329</v>
       </c>
-      <c r="I108" s="1">
+      <c r="I108" s="12">
         <v>0.29422718808193671</v>
       </c>
       <c r="K108">
@@ -4699,10 +4698,10 @@
       <c r="M108">
         <v>46424</v>
       </c>
-      <c r="O108" s="1">
+      <c r="O108" s="12">
         <v>0.78009219369291749</v>
       </c>
-      <c r="P108" s="1">
+      <c r="P108" s="12">
         <v>0.21990780630708254</v>
       </c>
     </row>
@@ -4719,10 +4718,10 @@
       <c r="F109">
         <v>529</v>
       </c>
-      <c r="H109" s="1">
+      <c r="H109" s="12">
         <v>0.77693761814744799</v>
       </c>
-      <c r="I109" s="1">
+      <c r="I109" s="12">
         <v>0.22306238185255198</v>
       </c>
       <c r="K109">
@@ -4734,10 +4733,10 @@
       <c r="M109">
         <v>46501</v>
       </c>
-      <c r="O109" s="1">
+      <c r="O109" s="12">
         <v>0.86802434356250402</v>
       </c>
-      <c r="P109" s="1">
+      <c r="P109" s="12">
         <v>0.13197565643749598</v>
       </c>
     </row>
@@ -4754,10 +4753,10 @@
       <c r="F110">
         <v>171</v>
       </c>
-      <c r="H110" s="1">
+      <c r="H110" s="12">
         <v>0.74853801169590639</v>
       </c>
-      <c r="I110" s="1">
+      <c r="I110" s="12">
         <v>0.25146198830409355</v>
       </c>
       <c r="K110">
@@ -4769,10 +4768,10 @@
       <c r="M110">
         <v>13485</v>
       </c>
-      <c r="O110" s="1">
+      <c r="O110" s="12">
         <v>0.81067853170189097</v>
       </c>
-      <c r="P110" s="1">
+      <c r="P110" s="12">
         <v>0.189321468298109</v>
       </c>
     </row>
@@ -4789,10 +4788,10 @@
       <c r="F111">
         <v>69</v>
       </c>
-      <c r="H111" s="1">
+      <c r="H111" s="12">
         <v>0.88405797101449279</v>
       </c>
-      <c r="I111" s="1">
+      <c r="I111" s="12">
         <v>0.11594202898550725</v>
       </c>
       <c r="K111">
@@ -4804,10 +4803,10 @@
       <c r="M111">
         <v>6367</v>
       </c>
-      <c r="O111" s="1">
+      <c r="O111" s="12">
         <v>0.93434898696403335</v>
       </c>
-      <c r="P111" s="1">
+      <c r="P111" s="12">
         <v>6.565101303596671E-2</v>
       </c>
     </row>
@@ -4824,10 +4823,10 @@
       <c r="F112">
         <v>160</v>
       </c>
-      <c r="H112" s="1">
+      <c r="H112" s="12">
         <v>0.88124999999999998</v>
       </c>
-      <c r="I112" s="1">
+      <c r="I112" s="12">
         <v>0.11874999999999999</v>
       </c>
       <c r="K112">
@@ -4839,10 +4838,10 @@
       <c r="M112">
         <v>16149</v>
       </c>
-      <c r="O112" s="1">
+      <c r="O112" s="12">
         <v>0.94755093194625051</v>
       </c>
-      <c r="P112" s="1">
+      <c r="P112" s="12">
         <v>5.2449068053749458E-2</v>
       </c>
     </row>
@@ -4859,10 +4858,10 @@
       <c r="F113">
         <v>209</v>
       </c>
-      <c r="H113" s="1">
+      <c r="H113" s="12">
         <v>0.75119617224880386</v>
       </c>
-      <c r="I113" s="1">
+      <c r="I113" s="12">
         <v>0.24880382775119617</v>
       </c>
       <c r="K113">
@@ -4874,10 +4873,10 @@
       <c r="M113">
         <v>17174</v>
       </c>
-      <c r="O113" s="1">
+      <c r="O113" s="12">
         <v>0.87201583789449166</v>
       </c>
-      <c r="P113" s="1">
+      <c r="P113" s="12">
         <v>0.12798416210550834</v>
       </c>
     </row>
@@ -4894,10 +4893,10 @@
       <c r="F114">
         <v>961</v>
       </c>
-      <c r="H114" s="1">
+      <c r="H114" s="12">
         <v>0.63475546305931319</v>
       </c>
-      <c r="I114" s="1">
+      <c r="I114" s="12">
         <v>0.36524453694068676</v>
       </c>
       <c r="K114">
@@ -4909,10 +4908,10 @@
       <c r="M114">
         <v>75474</v>
       </c>
-      <c r="O114" s="1">
+      <c r="O114" s="12">
         <v>0.7392082041497734</v>
       </c>
-      <c r="P114" s="1">
+      <c r="P114" s="12">
         <v>0.26079179585022655</v>
       </c>
     </row>
@@ -4921,34 +4920,34 @@
         <v>122</v>
       </c>
       <c r="D115">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="E115">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="F115">
         <v>432</v>
       </c>
-      <c r="H115" s="1">
-        <v>0.81018518518518523</v>
-      </c>
-      <c r="I115" s="1">
-        <v>0.18981481481481483</v>
+      <c r="H115" s="12">
+        <v>0.82870370370370372</v>
+      </c>
+      <c r="I115" s="12">
+        <v>0.17129629629629631</v>
       </c>
       <c r="K115">
-        <v>35596</v>
+        <v>36208</v>
       </c>
       <c r="L115">
-        <v>6323</v>
+        <v>5711</v>
       </c>
       <c r="M115">
         <v>41919</v>
       </c>
-      <c r="O115" s="1">
-        <v>0.84916147808869491</v>
-      </c>
-      <c r="P115" s="1">
-        <v>0.15083852191130515</v>
+      <c r="O115" s="12">
+        <v>0.86376106300245714</v>
+      </c>
+      <c r="P115" s="12">
+        <v>0.13623893699754289</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
@@ -4956,34 +4955,34 @@
         <v>123</v>
       </c>
       <c r="D116">
-        <v>281</v>
+        <v>320</v>
       </c>
       <c r="E116">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="F116">
         <v>496</v>
       </c>
-      <c r="H116" s="1">
-        <v>0.56653225806451613</v>
-      </c>
-      <c r="I116" s="1">
-        <v>0.43346774193548387</v>
+      <c r="H116" s="12">
+        <v>0.64516129032258063</v>
+      </c>
+      <c r="I116" s="12">
+        <v>0.35483870967741937</v>
       </c>
       <c r="K116">
-        <v>24988</v>
+        <v>27456</v>
       </c>
       <c r="L116">
-        <v>11205</v>
+        <v>8737</v>
       </c>
       <c r="M116">
         <v>36193</v>
       </c>
-      <c r="O116" s="1">
-        <v>0.69040974774127595</v>
-      </c>
-      <c r="P116" s="1">
-        <v>0.30959025225872405</v>
+      <c r="O116" s="12">
+        <v>0.75859972922940899</v>
+      </c>
+      <c r="P116" s="12">
+        <v>0.24140027077059101</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
@@ -4999,10 +4998,10 @@
       <c r="F117">
         <v>223</v>
       </c>
-      <c r="H117" s="1">
+      <c r="H117" s="12">
         <v>0.820627802690583</v>
       </c>
-      <c r="I117" s="1">
+      <c r="I117" s="12">
         <v>0.17937219730941703</v>
       </c>
       <c r="K117">
@@ -5014,10 +5013,10 @@
       <c r="M117">
         <v>17734</v>
       </c>
-      <c r="O117" s="1">
+      <c r="O117" s="12">
         <v>0.91406338107589935</v>
       </c>
-      <c r="P117" s="1">
+      <c r="P117" s="12">
         <v>8.5936618924100594E-2</v>
       </c>
     </row>
@@ -5034,10 +5033,10 @@
       <c r="F118">
         <v>85</v>
       </c>
-      <c r="H118" s="1">
+      <c r="H118" s="12">
         <v>0.84705882352941175</v>
       </c>
-      <c r="I118" s="1">
+      <c r="I118" s="12">
         <v>0.15294117647058825</v>
       </c>
       <c r="K118">
@@ -5049,10 +5048,10 @@
       <c r="M118">
         <v>7129</v>
       </c>
-      <c r="O118" s="1">
+      <c r="O118" s="12">
         <v>0.93687754243231869</v>
       </c>
-      <c r="P118" s="1">
+      <c r="P118" s="12">
         <v>6.3122457567681298E-2</v>
       </c>
     </row>
@@ -5069,10 +5068,10 @@
       <c r="F119">
         <v>87</v>
       </c>
-      <c r="H119" s="1">
+      <c r="H119" s="12">
         <v>0.8045977011494253</v>
       </c>
-      <c r="I119" s="1">
+      <c r="I119" s="12">
         <v>0.19540229885057472</v>
       </c>
       <c r="K119">
@@ -5084,10 +5083,10 @@
       <c r="M119">
         <v>7737</v>
       </c>
-      <c r="O119" s="1">
+      <c r="O119" s="12">
         <v>0.86493472922321313</v>
       </c>
-      <c r="P119" s="1">
+      <c r="P119" s="12">
         <v>0.13506527077678687</v>
       </c>
     </row>
@@ -5104,10 +5103,10 @@
       <c r="F120">
         <v>396</v>
       </c>
-      <c r="H120" s="1">
+      <c r="H120" s="12">
         <v>0.61363636363636365</v>
       </c>
-      <c r="I120" s="1">
+      <c r="I120" s="12">
         <v>0.38636363636363635</v>
       </c>
       <c r="K120">
@@ -5119,10 +5118,10 @@
       <c r="M120">
         <v>34997</v>
       </c>
-      <c r="O120" s="1">
+      <c r="O120" s="12">
         <v>0.69825985084435804</v>
       </c>
-      <c r="P120" s="1">
+      <c r="P120" s="12">
         <v>0.3017401491556419</v>
       </c>
     </row>
@@ -5139,10 +5138,10 @@
       <c r="F121">
         <v>212</v>
       </c>
-      <c r="H121" s="1">
+      <c r="H121" s="12">
         <v>0.68396226415094341</v>
       </c>
-      <c r="I121" s="1">
+      <c r="I121" s="12">
         <v>0.31603773584905659</v>
       </c>
       <c r="K121">
@@ -5154,10 +5153,10 @@
       <c r="M121">
         <v>15246</v>
       </c>
-      <c r="O121" s="1">
+      <c r="O121" s="12">
         <v>0.78709169618260533</v>
       </c>
-      <c r="P121" s="1">
+      <c r="P121" s="12">
         <v>0.21290830381739473</v>
       </c>
     </row>
@@ -5174,10 +5173,10 @@
       <c r="F122">
         <v>150</v>
       </c>
-      <c r="H122" s="1">
+      <c r="H122" s="12">
         <v>0.54666666666666663</v>
       </c>
-      <c r="I122" s="1">
+      <c r="I122" s="12">
         <v>0.45333333333333331</v>
       </c>
       <c r="K122">
@@ -5189,10 +5188,10 @@
       <c r="M122">
         <v>13900</v>
       </c>
-      <c r="O122" s="1">
+      <c r="O122" s="12">
         <v>0.60086330935251797</v>
       </c>
-      <c r="P122" s="1">
+      <c r="P122" s="12">
         <v>0.39913669064748203</v>
       </c>
     </row>
@@ -5209,10 +5208,10 @@
       <c r="F123">
         <v>126</v>
       </c>
-      <c r="H123" s="1">
+      <c r="H123" s="12">
         <v>0.83333333333333337</v>
       </c>
-      <c r="I123" s="1">
+      <c r="I123" s="12">
         <v>0.16666666666666666</v>
       </c>
       <c r="K123">
@@ -5224,10 +5223,10 @@
       <c r="M123">
         <v>11464</v>
       </c>
-      <c r="O123" s="1">
+      <c r="O123" s="12">
         <v>0.88625261688764834</v>
       </c>
-      <c r="P123" s="1">
+      <c r="P123" s="12">
         <v>0.1137473831123517</v>
       </c>
     </row>
@@ -5238,37 +5237,37 @@
       <c r="B124" s="13"/>
       <c r="C124" s="13"/>
       <c r="D124" s="13">
-        <v>7360</v>
+        <v>7427</v>
       </c>
       <c r="E124" s="13">
-        <v>3074</v>
+        <v>3007</v>
       </c>
       <c r="F124" s="13">
         <v>10434</v>
       </c>
       <c r="G124" s="13"/>
       <c r="H124" s="14">
-        <v>0.70538623730113093</v>
+        <v>0.71180755223308412</v>
       </c>
       <c r="I124" s="14">
-        <v>0.29461376269886907</v>
+        <v>0.28819244776691583</v>
       </c>
       <c r="J124" s="13"/>
       <c r="K124" s="13">
-        <v>688263</v>
+        <v>693214</v>
       </c>
       <c r="L124" s="13">
-        <v>181359</v>
+        <v>176408</v>
       </c>
       <c r="M124" s="13">
         <v>869622</v>
       </c>
       <c r="N124" s="13"/>
       <c r="O124" s="14">
-        <v>0.79145076826483229</v>
+        <v>0.79714404649376391</v>
       </c>
       <c r="P124" s="14">
-        <v>0.20854923173516771</v>
+        <v>0.20285595350623603</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
@@ -5287,10 +5286,10 @@
       <c r="F125">
         <v>143</v>
       </c>
-      <c r="H125" s="1">
+      <c r="H125" s="12">
         <v>0.71328671328671334</v>
       </c>
-      <c r="I125" s="1">
+      <c r="I125" s="12">
         <v>0.28671328671328672</v>
       </c>
       <c r="K125">
@@ -5302,10 +5301,10 @@
       <c r="M125">
         <v>11101</v>
       </c>
-      <c r="O125" s="1">
+      <c r="O125" s="12">
         <v>0.81037744347356089</v>
       </c>
-      <c r="P125" s="1">
+      <c r="P125" s="12">
         <v>0.18962255652643906</v>
       </c>
     </row>
@@ -5322,10 +5321,10 @@
       <c r="F126">
         <v>786</v>
       </c>
-      <c r="H126" s="1">
+      <c r="H126" s="12">
         <v>0.72137404580152675</v>
       </c>
-      <c r="I126" s="1">
+      <c r="I126" s="12">
         <v>0.2786259541984733</v>
       </c>
       <c r="K126">
@@ -5337,10 +5336,10 @@
       <c r="M126">
         <v>72662</v>
       </c>
-      <c r="O126" s="1">
+      <c r="O126" s="12">
         <v>0.79105997632875502</v>
       </c>
-      <c r="P126" s="1">
+      <c r="P126" s="12">
         <v>0.20894002367124495</v>
       </c>
     </row>
@@ -5357,10 +5356,10 @@
       <c r="F127">
         <v>533</v>
       </c>
-      <c r="H127" s="1">
+      <c r="H127" s="12">
         <v>0.58536585365853655</v>
       </c>
-      <c r="I127" s="1">
+      <c r="I127" s="12">
         <v>0.41463414634146339</v>
       </c>
       <c r="K127">
@@ -5372,10 +5371,10 @@
       <c r="M127">
         <v>41275</v>
       </c>
-      <c r="O127" s="1">
+      <c r="O127" s="12">
         <v>0.69749242883101148</v>
       </c>
-      <c r="P127" s="1">
+      <c r="P127" s="12">
         <v>0.30250757116898846</v>
       </c>
     </row>
@@ -5392,10 +5391,10 @@
       <c r="F128">
         <v>224</v>
       </c>
-      <c r="H128" s="1">
+      <c r="H128" s="12">
         <v>0.53125</v>
       </c>
-      <c r="I128" s="1">
+      <c r="I128" s="12">
         <v>0.46875</v>
       </c>
       <c r="K128">
@@ -5407,10 +5406,10 @@
       <c r="M128">
         <v>16985</v>
       </c>
-      <c r="O128" s="1">
+      <c r="O128" s="12">
         <v>0.69425964085958203</v>
       </c>
-      <c r="P128" s="1">
+      <c r="P128" s="12">
         <v>0.30574035914041803</v>
       </c>
     </row>
@@ -5427,10 +5426,10 @@
       <c r="F129">
         <v>209</v>
       </c>
-      <c r="H129" s="1">
+      <c r="H129" s="12">
         <v>0.78947368421052633</v>
       </c>
-      <c r="I129" s="1">
+      <c r="I129" s="12">
         <v>0.21052631578947367</v>
       </c>
       <c r="K129">
@@ -5442,10 +5441,10 @@
       <c r="M129">
         <v>17104</v>
       </c>
-      <c r="O129" s="1">
+      <c r="O129" s="12">
         <v>0.90078344246959774</v>
       </c>
-      <c r="P129" s="1">
+      <c r="P129" s="12">
         <v>9.9216557530402247E-2</v>
       </c>
     </row>
@@ -5462,10 +5461,10 @@
       <c r="F130">
         <v>482</v>
       </c>
-      <c r="H130" s="1">
+      <c r="H130" s="12">
         <v>0.68464730290456433</v>
       </c>
-      <c r="I130" s="1">
+      <c r="I130" s="12">
         <v>0.31535269709543567</v>
       </c>
       <c r="K130">
@@ -5477,10 +5476,10 @@
       <c r="M130">
         <v>39481</v>
       </c>
-      <c r="O130" s="1">
+      <c r="O130" s="12">
         <v>0.79574985436032519</v>
       </c>
-      <c r="P130" s="1">
+      <c r="P130" s="12">
         <v>0.20425014563967478</v>
       </c>
     </row>
@@ -5497,10 +5496,10 @@
       <c r="F131">
         <v>191</v>
       </c>
-      <c r="H131" s="1">
+      <c r="H131" s="12">
         <v>0.83246073298429324</v>
       </c>
-      <c r="I131" s="1">
+      <c r="I131" s="12">
         <v>0.16753926701570682</v>
       </c>
       <c r="K131">
@@ -5512,10 +5511,10 @@
       <c r="M131">
         <v>16401</v>
       </c>
-      <c r="O131" s="1">
+      <c r="O131" s="12">
         <v>0.90189622583988782</v>
       </c>
-      <c r="P131" s="1">
+      <c r="P131" s="12">
         <v>9.8103774160112192E-2</v>
       </c>
     </row>
@@ -5532,10 +5531,10 @@
       <c r="F132">
         <v>724</v>
       </c>
-      <c r="H132" s="1">
+      <c r="H132" s="12">
         <v>0.55939226519337015</v>
       </c>
-      <c r="I132" s="1">
+      <c r="I132" s="12">
         <v>0.44060773480662985</v>
       </c>
       <c r="K132">
@@ -5547,10 +5546,10 @@
       <c r="M132">
         <v>60386</v>
       </c>
-      <c r="O132" s="1">
+      <c r="O132" s="12">
         <v>0.65140926704865365</v>
       </c>
-      <c r="P132" s="1">
+      <c r="P132" s="12">
         <v>0.34859073295134635</v>
       </c>
     </row>
@@ -5567,10 +5566,10 @@
       <c r="F133">
         <v>308</v>
       </c>
-      <c r="H133" s="1">
+      <c r="H133" s="12">
         <v>0.66233766233766234</v>
       </c>
-      <c r="I133" s="1">
+      <c r="I133" s="12">
         <v>0.33766233766233766</v>
       </c>
       <c r="K133">
@@ -5582,10 +5581,10 @@
       <c r="M133">
         <v>22648</v>
       </c>
-      <c r="O133" s="1">
+      <c r="O133" s="12">
         <v>0.79896679618509359</v>
       </c>
-      <c r="P133" s="1">
+      <c r="P133" s="12">
         <v>0.20103320381490639</v>
       </c>
     </row>
@@ -5602,10 +5601,10 @@
       <c r="F134">
         <v>431</v>
       </c>
-      <c r="H134" s="1">
+      <c r="H134" s="12">
         <v>0.6589327146171694</v>
       </c>
-      <c r="I134" s="1">
+      <c r="I134" s="12">
         <v>0.34106728538283065</v>
       </c>
       <c r="K134">
@@ -5617,10 +5616,10 @@
       <c r="M134">
         <v>33911</v>
       </c>
-      <c r="O134" s="1">
+      <c r="O134" s="12">
         <v>0.78414083925569877</v>
       </c>
-      <c r="P134" s="1">
+      <c r="P134" s="12">
         <v>0.21585916074430125</v>
       </c>
     </row>
@@ -5637,10 +5636,10 @@
       <c r="F135">
         <v>454</v>
       </c>
-      <c r="H135" s="1">
+      <c r="H135" s="12">
         <v>0.73568281938325997</v>
       </c>
-      <c r="I135" s="1">
+      <c r="I135" s="12">
         <v>0.26431718061674009</v>
       </c>
       <c r="K135">
@@ -5652,10 +5651,10 @@
       <c r="M135">
         <v>30315</v>
       </c>
-      <c r="O135" s="1">
+      <c r="O135" s="12">
         <v>0.82507009731156189</v>
       </c>
-      <c r="P135" s="1">
+      <c r="P135" s="12">
         <v>0.17492990268843805</v>
       </c>
     </row>
@@ -5672,10 +5671,10 @@
       <c r="F136">
         <v>193</v>
       </c>
-      <c r="H136" s="1">
+      <c r="H136" s="12">
         <v>0.62176165803108807</v>
       </c>
-      <c r="I136" s="1">
+      <c r="I136" s="12">
         <v>0.37823834196891193</v>
       </c>
       <c r="K136">
@@ -5687,10 +5686,10 @@
       <c r="M136">
         <v>13600</v>
       </c>
-      <c r="O136" s="1">
+      <c r="O136" s="12">
         <v>0.75955882352941173</v>
       </c>
-      <c r="P136" s="1">
+      <c r="P136" s="12">
         <v>0.24044117647058824</v>
       </c>
     </row>
@@ -5707,10 +5706,10 @@
       <c r="F137">
         <v>295</v>
       </c>
-      <c r="H137" s="1">
+      <c r="H137" s="12">
         <v>0.72881355932203384</v>
       </c>
-      <c r="I137" s="1">
+      <c r="I137" s="12">
         <v>0.2711864406779661</v>
       </c>
       <c r="K137">
@@ -5722,10 +5721,10 @@
       <c r="M137">
         <v>24471</v>
       </c>
-      <c r="O137" s="1">
+      <c r="O137" s="12">
         <v>0.80985656491357116</v>
       </c>
-      <c r="P137" s="1">
+      <c r="P137" s="12">
         <v>0.19014343508642884</v>
       </c>
     </row>
@@ -5776,37 +5775,37 @@
       <c r="B139" s="13"/>
       <c r="C139" s="13"/>
       <c r="D139" s="13">
-        <v>37728</v>
+        <v>38086</v>
       </c>
       <c r="E139" s="13">
-        <v>28285</v>
+        <v>27927</v>
       </c>
       <c r="F139" s="13">
         <v>66013</v>
       </c>
       <c r="G139" s="13"/>
       <c r="H139" s="14">
-        <v>0.57152379076848503</v>
+        <v>0.57694696499174403</v>
       </c>
       <c r="I139" s="14">
-        <v>0.42847620923151503</v>
+        <v>0.42305303500825597</v>
       </c>
       <c r="J139" s="13"/>
       <c r="K139" s="13">
-        <v>3532098</v>
+        <v>3563752</v>
       </c>
       <c r="L139" s="13">
-        <v>1743839</v>
+        <v>1712185</v>
       </c>
       <c r="M139" s="13">
         <v>5275937</v>
       </c>
       <c r="N139" s="13"/>
       <c r="O139" s="14">
-        <v>0.66947311918243146</v>
+        <v>0.67547281174888929</v>
       </c>
       <c r="P139" s="14">
-        <v>0.33052688081756854</v>
+        <v>0.32452718825111065</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to county spreadsheets
</commit_message>
<xml_diff>
--- a/Locations/CountyStats.xlsx
+++ b/Locations/CountyStats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\Rainfall\DQ_Checks\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63FD83B6-E8EA-4819-A9E7-AD82F593FE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B235AF27-BBE2-435F-9C83-385062570405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49CB3039-2747-4D63-8D2F-D97935DF585E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1E6E5C9-CB94-454C-806C-B5DCCF60EE97}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -888,7 +888,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0157EE9D-9C37-49FF-BC35-F01517CEB7A6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689E0538-C2CB-43CD-BB5C-83E42C79E258}">
   <dimension ref="A1:P139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -902,12 +902,12 @@
   <cols>
     <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -1100,34 +1100,34 @@
         <v>10</v>
       </c>
       <c r="D7">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E7">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7">
         <v>113</v>
       </c>
       <c r="H7" s="1">
-        <v>0.62831858407079644</v>
+        <v>0.63716814159292035</v>
       </c>
       <c r="I7" s="1">
-        <v>0.37168141592920356</v>
+        <v>0.36283185840707965</v>
       </c>
       <c r="K7">
-        <v>6555</v>
+        <v>6651</v>
       </c>
       <c r="L7">
-        <v>1658</v>
+        <v>1562</v>
       </c>
       <c r="M7">
         <v>8213</v>
       </c>
       <c r="O7" s="1">
-        <v>0.79812492390113232</v>
+        <v>0.80981370997199564</v>
       </c>
       <c r="P7" s="1">
-        <v>0.20187507609886765</v>
+        <v>0.19018629002800438</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1172,37 +1172,37 @@
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E9" s="13">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F9" s="13">
         <v>246</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="14">
-        <v>0.491869918699187</v>
+        <v>0.49593495934959347</v>
       </c>
       <c r="I9" s="14">
-        <v>0.50813008130081305</v>
+        <v>0.50406504065040647</v>
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="13">
-        <v>10743</v>
+        <v>10839</v>
       </c>
       <c r="L9" s="13">
-        <v>6886</v>
+        <v>6790</v>
       </c>
       <c r="M9" s="13">
         <v>17629</v>
       </c>
       <c r="N9" s="13"/>
       <c r="O9" s="14">
-        <v>0.6093936127970957</v>
+        <v>0.61483918543309324</v>
       </c>
       <c r="P9" s="14">
-        <v>0.3906063872029043</v>
+        <v>0.38516081456690682</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1353,34 +1353,34 @@
         <v>18</v>
       </c>
       <c r="D14">
-        <v>814</v>
+        <v>822</v>
       </c>
       <c r="E14">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="F14">
         <v>1107</v>
       </c>
       <c r="H14" s="1">
-        <v>0.73532068654019878</v>
+        <v>0.74254742547425479</v>
       </c>
       <c r="I14" s="1">
-        <v>0.26467931345980128</v>
+        <v>0.25745257452574527</v>
       </c>
       <c r="K14">
-        <v>76754</v>
+        <v>77326</v>
       </c>
       <c r="L14">
-        <v>15605</v>
+        <v>15033</v>
       </c>
       <c r="M14">
         <v>92359</v>
       </c>
       <c r="O14" s="1">
-        <v>0.83103974707391803</v>
+        <v>0.83723297134009678</v>
       </c>
       <c r="P14" s="1">
-        <v>0.16896025292608191</v>
+        <v>0.1627670286599032</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1458,34 +1458,34 @@
         <v>21</v>
       </c>
       <c r="D17">
-        <v>877</v>
+        <v>881</v>
       </c>
       <c r="E17">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="F17">
         <v>1225</v>
       </c>
       <c r="H17" s="1">
-        <v>0.71591836734693881</v>
+        <v>0.71918367346938772</v>
       </c>
       <c r="I17" s="1">
-        <v>0.28408163265306124</v>
+        <v>0.28081632653061223</v>
       </c>
       <c r="K17">
-        <v>82847</v>
+        <v>83111</v>
       </c>
       <c r="L17">
-        <v>19916</v>
+        <v>19652</v>
       </c>
       <c r="M17">
         <v>102763</v>
       </c>
       <c r="O17" s="1">
-        <v>0.80619483666300129</v>
+        <v>0.80876385469478318</v>
       </c>
       <c r="P17" s="1">
-        <v>0.19380516333699874</v>
+        <v>0.19123614530521685</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
@@ -1493,34 +1493,34 @@
         <v>22</v>
       </c>
       <c r="D18">
-        <v>1476</v>
+        <v>1480</v>
       </c>
       <c r="E18">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="F18">
         <v>2551</v>
       </c>
       <c r="H18" s="1">
-        <v>0.5785966287730302</v>
+        <v>0.58016464131713052</v>
       </c>
       <c r="I18" s="1">
-        <v>0.4214033712269698</v>
+        <v>0.41983535868286948</v>
       </c>
       <c r="K18">
-        <v>133428</v>
+        <v>133740</v>
       </c>
       <c r="L18">
-        <v>60793</v>
+        <v>60481</v>
       </c>
       <c r="M18">
         <v>194221</v>
       </c>
       <c r="O18" s="1">
-        <v>0.6869905931902317</v>
+        <v>0.68859701062192036</v>
       </c>
       <c r="P18" s="1">
-        <v>0.31300940680976824</v>
+        <v>0.31140298937807959</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -1598,34 +1598,34 @@
         <v>25</v>
       </c>
       <c r="D21">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="E21">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F21">
         <v>1290</v>
       </c>
       <c r="H21" s="1">
-        <v>0.56279069767441858</v>
+        <v>0.56356589147286817</v>
       </c>
       <c r="I21" s="1">
-        <v>0.43720930232558142</v>
+        <v>0.43643410852713177</v>
       </c>
       <c r="K21">
-        <v>68815</v>
+        <v>68827</v>
       </c>
       <c r="L21">
-        <v>32668</v>
+        <v>32656</v>
       </c>
       <c r="M21">
         <v>101483</v>
       </c>
       <c r="O21" s="1">
-        <v>0.67809386793847248</v>
+        <v>0.67821211434427442</v>
       </c>
       <c r="P21" s="1">
-        <v>0.32190613206152757</v>
+        <v>0.32178788565572558</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -1668,34 +1668,34 @@
         <v>27</v>
       </c>
       <c r="D23">
-        <v>831</v>
+        <v>841</v>
       </c>
       <c r="E23">
-        <v>890</v>
+        <v>880</v>
       </c>
       <c r="F23">
         <v>1721</v>
       </c>
       <c r="H23" s="1">
-        <v>0.48285880302149914</v>
+        <v>0.48866937826844858</v>
       </c>
       <c r="I23" s="1">
-        <v>0.51714119697850092</v>
+        <v>0.51133062173155142</v>
       </c>
       <c r="K23">
-        <v>77005</v>
+        <v>77753</v>
       </c>
       <c r="L23">
-        <v>54066</v>
+        <v>53318</v>
       </c>
       <c r="M23">
         <v>131071</v>
       </c>
       <c r="O23" s="1">
-        <v>0.5875060081940322</v>
+        <v>0.59321283884306975</v>
       </c>
       <c r="P23" s="1">
-        <v>0.41249399180596774</v>
+        <v>0.4067871611569302</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
@@ -1878,34 +1878,34 @@
         <v>33</v>
       </c>
       <c r="D29">
-        <v>2252</v>
+        <v>2377</v>
       </c>
       <c r="E29">
-        <v>858</v>
+        <v>733</v>
       </c>
       <c r="F29">
         <v>3110</v>
       </c>
       <c r="H29" s="1">
-        <v>0.72411575562700969</v>
+        <v>0.7643086816720257</v>
       </c>
       <c r="I29" s="1">
-        <v>0.27588424437299036</v>
+        <v>0.23569131832797427</v>
       </c>
       <c r="K29">
-        <v>215024</v>
+        <v>225848</v>
       </c>
       <c r="L29">
-        <v>53405</v>
+        <v>42581</v>
       </c>
       <c r="M29">
         <v>268429</v>
       </c>
       <c r="O29" s="1">
-        <v>0.80104608667468868</v>
+        <v>0.84136959866482386</v>
       </c>
       <c r="P29" s="1">
-        <v>0.19895391332531134</v>
+        <v>0.15863040133517614</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
@@ -2053,34 +2053,34 @@
         <v>38</v>
       </c>
       <c r="D34">
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="E34">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="F34">
         <v>1141</v>
       </c>
       <c r="H34" s="1">
-        <v>0.57055214723926384</v>
+        <v>0.57405784399649429</v>
       </c>
       <c r="I34" s="1">
-        <v>0.42944785276073622</v>
+        <v>0.42594215600350571</v>
       </c>
       <c r="K34">
-        <v>58638</v>
+        <v>58978</v>
       </c>
       <c r="L34">
-        <v>28800</v>
+        <v>28460</v>
       </c>
       <c r="M34">
         <v>87438</v>
       </c>
       <c r="O34" s="1">
-        <v>0.67062375626157966</v>
+        <v>0.67451222580571379</v>
       </c>
       <c r="P34" s="1">
-        <v>0.32937624373842039</v>
+        <v>0.32548777419428626</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
@@ -2088,34 +2088,34 @@
         <v>39</v>
       </c>
       <c r="D35">
-        <v>480</v>
+        <v>488</v>
       </c>
       <c r="E35">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="F35">
         <v>784</v>
       </c>
       <c r="H35" s="1">
-        <v>0.61224489795918369</v>
+        <v>0.62244897959183676</v>
       </c>
       <c r="I35" s="1">
-        <v>0.38775510204081631</v>
+        <v>0.37755102040816324</v>
       </c>
       <c r="K35">
-        <v>44445</v>
+        <v>45201</v>
       </c>
       <c r="L35">
-        <v>18146</v>
+        <v>17390</v>
       </c>
       <c r="M35">
         <v>62591</v>
       </c>
       <c r="O35" s="1">
-        <v>0.71008611461711746</v>
+        <v>0.72216452844658174</v>
       </c>
       <c r="P35" s="1">
-        <v>0.28991388538288254</v>
+        <v>0.2778354715534182</v>
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
@@ -2263,34 +2263,34 @@
         <v>44</v>
       </c>
       <c r="D40">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E40">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F40">
         <v>670</v>
       </c>
       <c r="H40" s="1">
-        <v>0.71194029850746265</v>
+        <v>0.71343283582089556</v>
       </c>
       <c r="I40" s="1">
-        <v>0.28805970149253729</v>
+        <v>0.28656716417910449</v>
       </c>
       <c r="K40">
-        <v>41656</v>
+        <v>41664</v>
       </c>
       <c r="L40">
-        <v>7409</v>
+        <v>7401</v>
       </c>
       <c r="M40">
         <v>49065</v>
       </c>
       <c r="O40" s="1">
-        <v>0.84899622949149089</v>
+        <v>0.84915927850810147</v>
       </c>
       <c r="P40" s="1">
-        <v>0.15100377050850913</v>
+        <v>0.15084072149189851</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
@@ -2298,34 +2298,34 @@
         <v>45</v>
       </c>
       <c r="D41">
-        <v>899</v>
+        <v>910</v>
       </c>
       <c r="E41">
-        <v>1058</v>
+        <v>1047</v>
       </c>
       <c r="F41">
         <v>1957</v>
       </c>
       <c r="H41" s="1">
-        <v>0.45937659683188553</v>
+        <v>0.46499744506898316</v>
       </c>
       <c r="I41" s="1">
-        <v>0.54062340316811441</v>
+        <v>0.53500255493101689</v>
       </c>
       <c r="K41">
-        <v>83873</v>
+        <v>84485</v>
       </c>
       <c r="L41">
-        <v>62746</v>
+        <v>62134</v>
       </c>
       <c r="M41">
         <v>146619</v>
       </c>
       <c r="O41" s="1">
-        <v>0.57204727900203933</v>
+        <v>0.57622136285201786</v>
       </c>
       <c r="P41" s="1">
-        <v>0.42795272099796072</v>
+        <v>0.4237786371479822</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
@@ -2403,34 +2403,34 @@
         <v>48</v>
       </c>
       <c r="D44">
-        <v>892</v>
+        <v>921</v>
       </c>
       <c r="E44">
-        <v>1624</v>
+        <v>1595</v>
       </c>
       <c r="F44">
         <v>2516</v>
       </c>
       <c r="H44" s="1">
-        <v>0.35453100158982515</v>
+        <v>0.36605723370429255</v>
       </c>
       <c r="I44" s="1">
-        <v>0.64546899841017491</v>
+        <v>0.63394276629570745</v>
       </c>
       <c r="K44">
-        <v>83030</v>
+        <v>85353</v>
       </c>
       <c r="L44">
-        <v>102600</v>
+        <v>100277</v>
       </c>
       <c r="M44">
         <v>185630</v>
       </c>
       <c r="O44" s="1">
-        <v>0.44728761514841353</v>
+        <v>0.4598017561816517</v>
       </c>
       <c r="P44" s="1">
-        <v>0.55271238485158647</v>
+        <v>0.54019824381834836</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
@@ -2438,34 +2438,34 @@
         <v>49</v>
       </c>
       <c r="D45">
-        <v>1072</v>
+        <v>1131</v>
       </c>
       <c r="E45">
-        <v>1027</v>
+        <v>968</v>
       </c>
       <c r="F45">
         <v>2099</v>
       </c>
       <c r="H45" s="1">
-        <v>0.51071939018580281</v>
+        <v>0.53882801333968555</v>
       </c>
       <c r="I45" s="1">
-        <v>0.48928060981419724</v>
+        <v>0.46117198666031445</v>
       </c>
       <c r="K45">
-        <v>99054</v>
+        <v>103835</v>
       </c>
       <c r="L45">
-        <v>62320</v>
+        <v>57539</v>
       </c>
       <c r="M45">
         <v>161374</v>
       </c>
       <c r="O45" s="1">
-        <v>0.61381635207654273</v>
+        <v>0.64344318167734582</v>
       </c>
       <c r="P45" s="1">
-        <v>0.38618364792345733</v>
+        <v>0.35655681832265423</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
@@ -2543,34 +2543,34 @@
         <v>52</v>
       </c>
       <c r="D48">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="E48">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F48">
         <v>846</v>
       </c>
       <c r="H48" s="1">
-        <v>0.47872340425531917</v>
+        <v>0.48108747044917255</v>
       </c>
       <c r="I48" s="1">
-        <v>0.52127659574468088</v>
+        <v>0.51891252955082745</v>
       </c>
       <c r="K48">
-        <v>38259</v>
+        <v>38353</v>
       </c>
       <c r="L48">
-        <v>29105</v>
+        <v>29011</v>
       </c>
       <c r="M48">
         <v>67364</v>
       </c>
       <c r="O48" s="1">
-        <v>0.56794430259485784</v>
+        <v>0.56933970666825007</v>
       </c>
       <c r="P48" s="1">
-        <v>0.43205569740514221</v>
+        <v>0.43066029333174988</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -2683,34 +2683,34 @@
         <v>56</v>
       </c>
       <c r="D52">
-        <v>2871</v>
+        <v>2880</v>
       </c>
       <c r="E52">
-        <v>952</v>
+        <v>943</v>
       </c>
       <c r="F52">
         <v>3823</v>
       </c>
       <c r="H52" s="1">
-        <v>0.75098090504839132</v>
+        <v>0.75333507716453052</v>
       </c>
       <c r="I52" s="1">
-        <v>0.24901909495160868</v>
+        <v>0.24666492283546954</v>
       </c>
       <c r="K52">
-        <v>287754</v>
+        <v>288306</v>
       </c>
       <c r="L52">
-        <v>56590</v>
+        <v>56038</v>
       </c>
       <c r="M52">
         <v>344344</v>
       </c>
       <c r="O52" s="1">
-        <v>0.83565852751899261</v>
+        <v>0.83726157563366865</v>
       </c>
       <c r="P52" s="1">
-        <v>0.16434147248100736</v>
+        <v>0.16273842436633135</v>
       </c>
     </row>
     <row r="53" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2755,37 +2755,37 @@
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
       <c r="D54" s="13">
-        <v>28249</v>
+        <v>28524</v>
       </c>
       <c r="E54" s="13">
-        <v>18864</v>
+        <v>18589</v>
       </c>
       <c r="F54" s="13">
         <v>47113</v>
       </c>
       <c r="G54" s="13"/>
       <c r="H54" s="14">
-        <v>0.59960095939549596</v>
+        <v>0.6054379895145714</v>
       </c>
       <c r="I54" s="14">
-        <v>0.40039904060450404</v>
+        <v>0.39456201048542866</v>
       </c>
       <c r="J54" s="13"/>
       <c r="K54" s="13">
-        <v>2641810</v>
+        <v>2664008</v>
       </c>
       <c r="L54" s="13">
-        <v>1098904</v>
+        <v>1076706</v>
       </c>
       <c r="M54" s="13">
         <v>3740714</v>
       </c>
       <c r="N54" s="13"/>
       <c r="O54" s="14">
-        <v>0.7062314841498174</v>
+        <v>0.71216564538213822</v>
       </c>
       <c r="P54" s="14">
-        <v>0.2937685158501826</v>
+        <v>0.28783435461786172</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -2796,34 +2796,34 @@
         <v>60</v>
       </c>
       <c r="D55">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E55">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F55">
         <v>285</v>
       </c>
       <c r="H55" s="1">
-        <v>0.85263157894736841</v>
+        <v>0.85614035087719298</v>
       </c>
       <c r="I55" s="1">
-        <v>0.14736842105263157</v>
+        <v>0.14385964912280702</v>
       </c>
       <c r="K55">
-        <v>21301</v>
+        <v>21327</v>
       </c>
       <c r="L55">
-        <v>1625</v>
+        <v>1599</v>
       </c>
       <c r="M55">
         <v>22926</v>
       </c>
       <c r="O55" s="1">
-        <v>0.92911977667277323</v>
+        <v>0.93025386024600887</v>
       </c>
       <c r="P55" s="1">
-        <v>7.0880223327226724E-2</v>
+        <v>6.9746139753991104E-2</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -3008,37 +3008,37 @@
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
       <c r="D61" s="13">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="E61" s="13">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F61" s="13">
         <v>943</v>
       </c>
       <c r="G61" s="13"/>
       <c r="H61" s="14">
-        <v>0.70307529162248139</v>
+        <v>0.70413573700954402</v>
       </c>
       <c r="I61" s="14">
-        <v>0.29692470837751855</v>
+        <v>0.29586426299045598</v>
       </c>
       <c r="J61" s="13"/>
       <c r="K61" s="13">
-        <v>59435</v>
+        <v>59461</v>
       </c>
       <c r="L61" s="13">
-        <v>16124</v>
+        <v>16098</v>
       </c>
       <c r="M61" s="13">
         <v>75559</v>
       </c>
       <c r="N61" s="13"/>
       <c r="O61" s="14">
-        <v>0.7866038460011382</v>
+        <v>0.78694794796119594</v>
       </c>
       <c r="P61" s="14">
-        <v>0.2133961539988618</v>
+        <v>0.21305205203880412</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -3924,34 +3924,34 @@
         <v>93</v>
       </c>
       <c r="D87">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="E87">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F87">
         <v>113</v>
       </c>
       <c r="H87" s="1">
-        <v>0.38053097345132741</v>
+        <v>0.4247787610619469</v>
       </c>
       <c r="I87" s="1">
-        <v>0.61946902654867253</v>
+        <v>0.5752212389380531</v>
       </c>
       <c r="K87">
-        <v>3810</v>
+        <v>4266</v>
       </c>
       <c r="L87">
-        <v>4519</v>
+        <v>4063</v>
       </c>
       <c r="M87">
         <v>8329</v>
       </c>
       <c r="O87" s="1">
-        <v>0.45743786769119943</v>
+        <v>0.51218633689518545</v>
       </c>
       <c r="P87" s="1">
-        <v>0.54256213230880057</v>
+        <v>0.4878136631048145</v>
       </c>
     </row>
     <row r="88" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3961,37 +3961,37 @@
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
       <c r="D88" s="13">
-        <v>838</v>
+        <v>843</v>
       </c>
       <c r="E88" s="13">
-        <v>1311</v>
+        <v>1306</v>
       </c>
       <c r="F88" s="13">
         <v>2149</v>
       </c>
       <c r="G88" s="13"/>
       <c r="H88" s="14">
-        <v>0.38994881340158211</v>
+        <v>0.39227547696603071</v>
       </c>
       <c r="I88" s="14">
-        <v>0.61005118659841784</v>
+        <v>0.60772452303396929</v>
       </c>
       <c r="J88" s="13"/>
       <c r="K88" s="13">
-        <v>75851</v>
+        <v>76307</v>
       </c>
       <c r="L88" s="13">
-        <v>83746</v>
+        <v>83290</v>
       </c>
       <c r="M88" s="13">
         <v>159597</v>
       </c>
       <c r="N88" s="13"/>
       <c r="O88" s="14">
-        <v>0.47526582579873056</v>
+        <v>0.47812302236257576</v>
       </c>
       <c r="P88" s="14">
-        <v>0.52473417420126944</v>
+        <v>0.52187697763742424</v>
       </c>
     </row>
     <row r="89" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4080,34 +4080,34 @@
         <v>98</v>
       </c>
       <c r="D91">
-        <v>317</v>
+        <v>378</v>
       </c>
       <c r="E91">
-        <v>164</v>
+        <v>103</v>
       </c>
       <c r="F91">
         <v>481</v>
       </c>
       <c r="H91" s="1">
-        <v>0.65904365904365902</v>
+        <v>0.78586278586278591</v>
       </c>
       <c r="I91" s="1">
-        <v>0.34095634095634098</v>
+        <v>0.21413721413721415</v>
       </c>
       <c r="K91">
-        <v>29238</v>
+        <v>34401</v>
       </c>
       <c r="L91">
-        <v>9436</v>
+        <v>4273</v>
       </c>
       <c r="M91">
         <v>38674</v>
       </c>
       <c r="O91" s="1">
-        <v>0.75601179086724934</v>
+        <v>0.88951233386771478</v>
       </c>
       <c r="P91" s="1">
-        <v>0.24398820913275068</v>
+        <v>0.11048766613228525</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
@@ -4185,34 +4185,34 @@
         <v>101</v>
       </c>
       <c r="D94">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="E94">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F94">
         <v>669</v>
       </c>
       <c r="H94" s="1">
-        <v>0.78026905829596416</v>
+        <v>0.78624813153961137</v>
       </c>
       <c r="I94" s="1">
-        <v>0.21973094170403587</v>
+        <v>0.21375186846038863</v>
       </c>
       <c r="K94">
-        <v>49352</v>
+        <v>49736</v>
       </c>
       <c r="L94">
-        <v>8315</v>
+        <v>7931</v>
       </c>
       <c r="M94">
         <v>57667</v>
       </c>
       <c r="O94" s="1">
-        <v>0.8558100820226473</v>
+        <v>0.86246900306934637</v>
       </c>
       <c r="P94" s="1">
-        <v>0.14418991797735273</v>
+        <v>0.13753099693065357</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
@@ -4395,34 +4395,34 @@
         <v>107</v>
       </c>
       <c r="D100">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E100">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F100">
         <v>365</v>
       </c>
       <c r="H100" s="1">
-        <v>0.75342465753424659</v>
+        <v>0.75616438356164384</v>
       </c>
       <c r="I100" s="1">
-        <v>0.24657534246575341</v>
+        <v>0.24383561643835616</v>
       </c>
       <c r="K100">
-        <v>22984</v>
+        <v>23042</v>
       </c>
       <c r="L100">
-        <v>3851</v>
+        <v>3793</v>
       </c>
       <c r="M100">
         <v>26835</v>
       </c>
       <c r="O100" s="1">
-        <v>0.856493385504006</v>
+        <v>0.85865474194149427</v>
       </c>
       <c r="P100" s="1">
-        <v>0.14350661449599403</v>
+        <v>0.14134525805850567</v>
       </c>
     </row>
     <row r="101" spans="2:16" x14ac:dyDescent="0.25">
@@ -4535,34 +4535,34 @@
         <v>111</v>
       </c>
       <c r="D104">
-        <v>618</v>
+        <v>693</v>
       </c>
       <c r="E104">
-        <v>275</v>
+        <v>200</v>
       </c>
       <c r="F104">
         <v>893</v>
       </c>
       <c r="H104" s="1">
-        <v>0.69204927211646139</v>
+        <v>0.77603583426651734</v>
       </c>
       <c r="I104" s="1">
-        <v>0.30795072788353861</v>
+        <v>0.22396416573348266</v>
       </c>
       <c r="K104">
-        <v>54466</v>
+        <v>60673</v>
       </c>
       <c r="L104">
-        <v>14863</v>
+        <v>8656</v>
       </c>
       <c r="M104">
         <v>69329</v>
       </c>
       <c r="O104" s="1">
-        <v>0.78561640871785254</v>
+        <v>0.87514604278151997</v>
       </c>
       <c r="P104" s="1">
-        <v>0.21438359128214743</v>
+        <v>0.12485395721848</v>
       </c>
     </row>
     <row r="105" spans="2:16" x14ac:dyDescent="0.25">
@@ -4675,34 +4675,34 @@
         <v>115</v>
       </c>
       <c r="D108">
-        <v>381</v>
+        <v>466</v>
       </c>
       <c r="E108">
-        <v>156</v>
+        <v>73</v>
       </c>
       <c r="F108">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="H108" s="1">
-        <v>0.70949720670391059</v>
+        <v>0.86456400742115025</v>
       </c>
       <c r="I108" s="1">
-        <v>0.29050279329608941</v>
+        <v>0.13543599257884972</v>
       </c>
       <c r="K108">
-        <v>36393</v>
+        <v>43549</v>
       </c>
       <c r="L108">
-        <v>10031</v>
+        <v>3055</v>
       </c>
       <c r="M108">
-        <v>46424</v>
+        <v>46604</v>
       </c>
       <c r="O108" s="1">
-        <v>0.78392641737032565</v>
+        <v>0.93444768689382884</v>
       </c>
       <c r="P108" s="1">
-        <v>0.2160735826296743</v>
+        <v>6.5552313106171142E-2</v>
       </c>
     </row>
     <row r="109" spans="2:16" x14ac:dyDescent="0.25">
@@ -4850,34 +4850,34 @@
         <v>120</v>
       </c>
       <c r="D113">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="E113">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="F113">
         <v>209</v>
       </c>
       <c r="H113" s="1">
-        <v>0.75119617224880386</v>
+        <v>0.82296650717703346</v>
       </c>
       <c r="I113" s="1">
-        <v>0.24880382775119617</v>
+        <v>0.17703349282296652</v>
       </c>
       <c r="K113">
-        <v>14976</v>
+        <v>16137</v>
       </c>
       <c r="L113">
-        <v>2198</v>
+        <v>1037</v>
       </c>
       <c r="M113">
         <v>17174</v>
       </c>
       <c r="O113" s="1">
-        <v>0.87201583789449166</v>
+        <v>0.93961802725049492</v>
       </c>
       <c r="P113" s="1">
-        <v>0.12798416210550834</v>
+        <v>6.0381972749505068E-2</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
@@ -4885,34 +4885,34 @@
         <v>121</v>
       </c>
       <c r="D114">
-        <v>613</v>
+        <v>630</v>
       </c>
       <c r="E114">
-        <v>348</v>
+        <v>331</v>
       </c>
       <c r="F114">
         <v>961</v>
       </c>
       <c r="H114" s="1">
-        <v>0.63787721123829344</v>
+        <v>0.65556711758584807</v>
       </c>
       <c r="I114" s="1">
-        <v>0.36212278876170656</v>
+        <v>0.34443288241415193</v>
       </c>
       <c r="K114">
-        <v>55975</v>
+        <v>57022</v>
       </c>
       <c r="L114">
-        <v>19499</v>
+        <v>18452</v>
       </c>
       <c r="M114">
         <v>75474</v>
       </c>
       <c r="O114" s="1">
-        <v>0.74164612979304134</v>
+        <v>0.75551845668707107</v>
       </c>
       <c r="P114" s="1">
-        <v>0.25835387020695871</v>
+        <v>0.24448154331292896</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
@@ -4923,31 +4923,31 @@
         <v>363</v>
       </c>
       <c r="E115">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F115">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H115" s="1">
-        <v>0.84027777777777779</v>
+        <v>0.84418604651162787</v>
       </c>
       <c r="I115" s="1">
-        <v>0.15972222222222221</v>
+        <v>0.1558139534883721</v>
       </c>
       <c r="K115">
         <v>36747</v>
       </c>
       <c r="L115">
-        <v>5172</v>
+        <v>4992</v>
       </c>
       <c r="M115">
-        <v>41919</v>
+        <v>41739</v>
       </c>
       <c r="O115" s="1">
-        <v>0.87661919416016598</v>
+        <v>0.88039962624883206</v>
       </c>
       <c r="P115" s="1">
-        <v>0.12338080583983396</v>
+        <v>0.11960037375116797</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
@@ -4955,34 +4955,34 @@
         <v>123</v>
       </c>
       <c r="D116">
-        <v>320</v>
+        <v>354</v>
       </c>
       <c r="E116">
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="F116">
         <v>496</v>
       </c>
       <c r="H116" s="1">
-        <v>0.64516129032258063</v>
+        <v>0.71370967741935487</v>
       </c>
       <c r="I116" s="1">
-        <v>0.35483870967741937</v>
+        <v>0.28629032258064518</v>
       </c>
       <c r="K116">
-        <v>27456</v>
+        <v>30345</v>
       </c>
       <c r="L116">
-        <v>8737</v>
+        <v>5848</v>
       </c>
       <c r="M116">
         <v>36193</v>
       </c>
       <c r="O116" s="1">
-        <v>0.75859972922940899</v>
+        <v>0.83842179426961017</v>
       </c>
       <c r="P116" s="1">
-        <v>0.24140027077059101</v>
+        <v>0.16157820573038986</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
@@ -4990,34 +4990,34 @@
         <v>124</v>
       </c>
       <c r="D117">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E117">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F117">
         <v>223</v>
       </c>
       <c r="H117" s="1">
-        <v>0.820627802690583</v>
+        <v>0.83856502242152464</v>
       </c>
       <c r="I117" s="1">
-        <v>0.17937219730941703</v>
+        <v>0.16143497757847533</v>
       </c>
       <c r="K117">
-        <v>16210</v>
+        <v>16501</v>
       </c>
       <c r="L117">
-        <v>1524</v>
+        <v>1233</v>
       </c>
       <c r="M117">
         <v>17734</v>
       </c>
       <c r="O117" s="1">
-        <v>0.91406338107589935</v>
+        <v>0.93047253862636747</v>
       </c>
       <c r="P117" s="1">
-        <v>8.5936618924100594E-2</v>
+        <v>6.9527461373632568E-2</v>
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
@@ -5025,34 +5025,34 @@
         <v>125</v>
       </c>
       <c r="D118">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E118">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F118">
         <v>85</v>
       </c>
       <c r="H118" s="1">
-        <v>0.84705882352941175</v>
+        <v>0.88235294117647056</v>
       </c>
       <c r="I118" s="1">
-        <v>0.15294117647058825</v>
+        <v>0.11764705882352941</v>
       </c>
       <c r="K118">
-        <v>6679</v>
+        <v>6857</v>
       </c>
       <c r="L118">
-        <v>450</v>
+        <v>272</v>
       </c>
       <c r="M118">
         <v>7129</v>
       </c>
       <c r="O118" s="1">
-        <v>0.93687754243231869</v>
+        <v>0.96184598120353482</v>
       </c>
       <c r="P118" s="1">
-        <v>6.3122457567681298E-2</v>
+        <v>3.8154018796465142E-2</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
@@ -5237,37 +5237,37 @@
       <c r="B124" s="13"/>
       <c r="C124" s="13"/>
       <c r="D124" s="13">
-        <v>7727</v>
+        <v>8026</v>
       </c>
       <c r="E124" s="13">
-        <v>2707</v>
+        <v>2408</v>
       </c>
       <c r="F124" s="13">
         <v>10434</v>
       </c>
       <c r="G124" s="13"/>
       <c r="H124" s="14">
-        <v>0.74055970864481502</v>
+        <v>0.76921602453517346</v>
       </c>
       <c r="I124" s="14">
-        <v>0.25944029135518498</v>
+        <v>0.23078397546482654</v>
       </c>
       <c r="J124" s="13"/>
       <c r="K124" s="13">
-        <v>719828</v>
+        <v>744362</v>
       </c>
       <c r="L124" s="13">
-        <v>149794</v>
+        <v>125260</v>
       </c>
       <c r="M124" s="13">
         <v>869622</v>
       </c>
       <c r="N124" s="13"/>
       <c r="O124" s="14">
-        <v>0.82774814804593255</v>
+        <v>0.85596040578550225</v>
       </c>
       <c r="P124" s="14">
-        <v>0.17225185195406739</v>
+        <v>0.1440395942144978</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
@@ -5558,34 +5558,34 @@
         <v>141</v>
       </c>
       <c r="D133">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E133">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F133">
         <v>308</v>
       </c>
       <c r="H133" s="1">
-        <v>0.72402597402597402</v>
+        <v>0.72077922077922074</v>
       </c>
       <c r="I133" s="1">
-        <v>0.27597402597402598</v>
+        <v>0.2792207792207792</v>
       </c>
       <c r="K133">
-        <v>19609</v>
+        <v>19561</v>
       </c>
       <c r="L133">
-        <v>3039</v>
+        <v>3087</v>
       </c>
       <c r="M133">
         <v>22648</v>
       </c>
       <c r="O133" s="1">
-        <v>0.865815966089721</v>
+        <v>0.8636965736488873</v>
       </c>
       <c r="P133" s="1">
-        <v>0.13418403391027905</v>
+        <v>0.13630342635111267</v>
       </c>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
@@ -5735,37 +5735,37 @@
       <c r="B138" s="13"/>
       <c r="C138" s="13"/>
       <c r="D138" s="13">
-        <v>3497</v>
+        <v>3496</v>
       </c>
       <c r="E138" s="13">
-        <v>1476</v>
+        <v>1477</v>
       </c>
       <c r="F138" s="13">
         <v>4973</v>
       </c>
       <c r="G138" s="13"/>
       <c r="H138" s="14">
-        <v>0.70319726523225412</v>
+        <v>0.70299617936859038</v>
       </c>
       <c r="I138" s="14">
-        <v>0.29680273476774582</v>
+        <v>0.29700382063140962</v>
       </c>
       <c r="J138" s="13"/>
       <c r="K138" s="13">
-        <v>324898</v>
+        <v>324850</v>
       </c>
       <c r="L138" s="13">
-        <v>75442</v>
+        <v>75490</v>
       </c>
       <c r="M138" s="13">
         <v>400340</v>
       </c>
       <c r="N138" s="13"/>
       <c r="O138" s="14">
-        <v>0.81155517809861621</v>
+        <v>0.81143528001198983</v>
       </c>
       <c r="P138" s="14">
-        <v>0.18844482190138381</v>
+        <v>0.18856471998801019</v>
       </c>
     </row>
     <row r="139" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5775,37 +5775,37 @@
       <c r="B139" s="13"/>
       <c r="C139" s="13"/>
       <c r="D139" s="13">
-        <v>41187</v>
+        <v>41767</v>
       </c>
       <c r="E139" s="13">
-        <v>24826</v>
+        <v>24246</v>
       </c>
       <c r="F139" s="13">
         <v>66013</v>
       </c>
       <c r="G139" s="13"/>
       <c r="H139" s="14">
-        <v>0.62392256070773944</v>
+        <v>0.6327087088906731</v>
       </c>
       <c r="I139" s="14">
-        <v>0.37607743929226062</v>
+        <v>0.36729129110932696</v>
       </c>
       <c r="J139" s="13"/>
       <c r="K139" s="13">
-        <v>3841512</v>
+        <v>3888774</v>
       </c>
       <c r="L139" s="13">
-        <v>1434425</v>
+        <v>1387163</v>
       </c>
       <c r="M139" s="13">
         <v>5275937</v>
       </c>
       <c r="N139" s="13"/>
       <c r="O139" s="14">
-        <v>0.72811938429135903</v>
+        <v>0.73707741392666359</v>
       </c>
       <c r="P139" s="14">
-        <v>0.27188061570864097</v>
+        <v>0.26292258607333635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refreshed following RR GitHub updates
</commit_message>
<xml_diff>
--- a/Locations/CountyStats.xlsx
+++ b/Locations/CountyStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\Rainfall\DQ_Checks\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58348AF9-6CB2-4713-95E9-8F714C106A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4D60070F-AD50-45C8-B790-022F211A78C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C23ACF87-5486-4EC6-AABF-B0E398C54656}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0ECB3BA4-2CF0-4D19-878A-BF5271E0FA6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -888,27 +889,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0F56FF-E59E-49CC-9AF7-A40BB59D9D57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898551F8-88C9-4B03-B821-DAF4E21B8F1C}">
   <dimension ref="A1:P139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5703125" customWidth="1"/>
-    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.140625" style="1" bestFit="1" customWidth="1"/>
@@ -1036,34 +1037,34 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="E5">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="F5">
         <v>113</v>
       </c>
       <c r="H5" s="1">
-        <v>0.45132743362831856</v>
+        <v>0.61946902654867253</v>
       </c>
       <c r="I5" s="1">
-        <v>0.54867256637168138</v>
+        <v>0.38053097345132741</v>
       </c>
       <c r="K5">
-        <v>4343</v>
+        <v>5898</v>
       </c>
       <c r="L5">
-        <v>3382</v>
+        <v>1827</v>
       </c>
       <c r="M5">
         <v>7725</v>
       </c>
       <c r="O5" s="1">
-        <v>0.56220064724919094</v>
+        <v>0.76349514563106791</v>
       </c>
       <c r="P5" s="1">
-        <v>0.43779935275080906</v>
+        <v>0.23650485436893204</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1166,37 +1167,37 @@
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13">
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="E9" s="13">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="F9" s="13">
         <v>246</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="14">
-        <v>0.58943089430894313</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I9" s="14">
-        <v>0.41056910569105692</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="13">
-        <v>12865</v>
+        <v>14420</v>
       </c>
       <c r="L9" s="13">
-        <v>4764</v>
+        <v>3209</v>
       </c>
       <c r="M9" s="13">
         <v>17629</v>
       </c>
       <c r="N9" s="13"/>
       <c r="O9" s="14">
-        <v>0.72976345793862385</v>
+        <v>0.81797038969879177</v>
       </c>
       <c r="P9" s="14">
-        <v>0.27023654206137615</v>
+        <v>0.18202961030120823</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1347,34 +1348,34 @@
         <v>18</v>
       </c>
       <c r="D14">
-        <v>822</v>
+        <v>871</v>
       </c>
       <c r="E14">
-        <v>285</v>
+        <v>236</v>
       </c>
       <c r="F14">
         <v>1107</v>
       </c>
       <c r="H14" s="1">
-        <v>0.74254742547425479</v>
+        <v>0.78681120144534777</v>
       </c>
       <c r="I14" s="1">
-        <v>0.25745257452574527</v>
+        <v>0.21318879855465223</v>
       </c>
       <c r="K14">
-        <v>77326</v>
+        <v>81723</v>
       </c>
       <c r="L14">
-        <v>15033</v>
+        <v>10636</v>
       </c>
       <c r="M14">
         <v>92359</v>
       </c>
       <c r="O14" s="1">
-        <v>0.83723297134009678</v>
+        <v>0.88484067605755801</v>
       </c>
       <c r="P14" s="1">
-        <v>0.1627670286599032</v>
+        <v>0.11515932394244199</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1382,34 +1383,34 @@
         <v>19</v>
       </c>
       <c r="D15">
-        <v>631</v>
+        <v>654</v>
       </c>
       <c r="E15">
-        <v>342</v>
+        <v>319</v>
       </c>
       <c r="F15">
         <v>973</v>
       </c>
       <c r="H15" s="1">
-        <v>0.64850976361767732</v>
+        <v>0.67214799588900309</v>
       </c>
       <c r="I15" s="1">
-        <v>0.35149023638232274</v>
+        <v>0.32785200411099691</v>
       </c>
       <c r="K15">
-        <v>56634</v>
+        <v>58526</v>
       </c>
       <c r="L15">
-        <v>17742</v>
+        <v>15850</v>
       </c>
       <c r="M15">
         <v>74376</v>
       </c>
       <c r="O15" s="1">
-        <v>0.76145530816392382</v>
+        <v>0.78689362159836507</v>
       </c>
       <c r="P15" s="1">
-        <v>0.23854469183607616</v>
+        <v>0.21310637840163493</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -1417,34 +1418,34 @@
         <v>20</v>
       </c>
       <c r="D16">
-        <v>849</v>
+        <v>876</v>
       </c>
       <c r="E16">
-        <v>235</v>
+        <v>208</v>
       </c>
       <c r="F16">
         <v>1084</v>
       </c>
       <c r="H16" s="1">
-        <v>0.78321033210332103</v>
+        <v>0.80811808118081185</v>
       </c>
       <c r="I16" s="1">
-        <v>0.21678966789667897</v>
+        <v>0.1918819188191882</v>
       </c>
       <c r="K16">
-        <v>71629</v>
+        <v>73242</v>
       </c>
       <c r="L16">
-        <v>10851</v>
+        <v>9238</v>
       </c>
       <c r="M16">
         <v>82480</v>
       </c>
       <c r="O16" s="1">
-        <v>0.86844083414161011</v>
+        <v>0.88799709020368578</v>
       </c>
       <c r="P16" s="1">
-        <v>0.13155916585838992</v>
+        <v>0.11200290979631426</v>
       </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
@@ -1452,34 +1453,34 @@
         <v>21</v>
       </c>
       <c r="D17">
-        <v>887</v>
+        <v>973</v>
       </c>
       <c r="E17">
-        <v>338</v>
+        <v>252</v>
       </c>
       <c r="F17">
         <v>1225</v>
       </c>
       <c r="H17" s="1">
-        <v>0.72408163265306125</v>
+        <v>0.79428571428571426</v>
       </c>
       <c r="I17" s="1">
-        <v>0.27591836734693875</v>
+        <v>0.20571428571428571</v>
       </c>
       <c r="K17">
-        <v>83474</v>
+        <v>90007</v>
       </c>
       <c r="L17">
-        <v>19289</v>
+        <v>12756</v>
       </c>
       <c r="M17">
         <v>102763</v>
       </c>
       <c r="O17" s="1">
-        <v>0.81229625448848319</v>
+        <v>0.8758697196461761</v>
       </c>
       <c r="P17" s="1">
-        <v>0.18770374551151678</v>
+        <v>0.12413028035382384</v>
       </c>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
@@ -1487,34 +1488,34 @@
         <v>22</v>
       </c>
       <c r="D18">
-        <v>1597</v>
+        <v>1675</v>
       </c>
       <c r="E18">
-        <v>954</v>
+        <v>876</v>
       </c>
       <c r="F18">
         <v>2551</v>
       </c>
       <c r="H18" s="1">
-        <v>0.62602900823206586</v>
+        <v>0.65660525284202276</v>
       </c>
       <c r="I18" s="1">
-        <v>0.37397099176793414</v>
+        <v>0.34339474715797724</v>
       </c>
       <c r="K18">
-        <v>144290</v>
+        <v>150882</v>
       </c>
       <c r="L18">
-        <v>49931</v>
+        <v>43339</v>
       </c>
       <c r="M18">
         <v>194221</v>
       </c>
       <c r="O18" s="1">
-        <v>0.74291657441780246</v>
+        <v>0.77685729143604454</v>
       </c>
       <c r="P18" s="1">
-        <v>0.2570834255821976</v>
+        <v>0.22314270856395549</v>
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
@@ -1522,34 +1523,34 @@
         <v>23</v>
       </c>
       <c r="D19">
-        <v>559</v>
+        <v>597</v>
       </c>
       <c r="E19">
-        <v>397</v>
+        <v>359</v>
       </c>
       <c r="F19">
         <v>956</v>
       </c>
       <c r="H19" s="1">
-        <v>0.58472803347280333</v>
+        <v>0.62447698744769875</v>
       </c>
       <c r="I19" s="1">
-        <v>0.41527196652719667</v>
+        <v>0.37552301255230125</v>
       </c>
       <c r="K19">
-        <v>50393</v>
+        <v>53645</v>
       </c>
       <c r="L19">
-        <v>20598</v>
+        <v>17346</v>
       </c>
       <c r="M19">
         <v>70991</v>
       </c>
       <c r="O19" s="1">
-        <v>0.70985054443521012</v>
+        <v>0.75565916806355737</v>
       </c>
       <c r="P19" s="1">
-        <v>0.29014945556478988</v>
+        <v>0.24434083193644265</v>
       </c>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
@@ -1662,34 +1663,34 @@
         <v>27</v>
       </c>
       <c r="D23">
-        <v>1016</v>
+        <v>1071</v>
       </c>
       <c r="E23">
-        <v>704</v>
+        <v>649</v>
       </c>
       <c r="F23">
         <v>1720</v>
       </c>
       <c r="H23" s="1">
-        <v>0.59069767441860466</v>
+        <v>0.62267441860465111</v>
       </c>
       <c r="I23" s="1">
-        <v>0.40930232558139534</v>
+        <v>0.37732558139534883</v>
       </c>
       <c r="K23">
-        <v>92580</v>
+        <v>97342</v>
       </c>
       <c r="L23">
-        <v>38479</v>
+        <v>33717</v>
       </c>
       <c r="M23">
         <v>131059</v>
       </c>
       <c r="O23" s="1">
-        <v>0.70639940790025868</v>
+        <v>0.74273418841895633</v>
       </c>
       <c r="P23" s="1">
-        <v>0.29360059209974132</v>
+        <v>0.25726581158104367</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
@@ -1697,34 +1698,34 @@
         <v>28</v>
       </c>
       <c r="D24">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="E24">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F24">
         <v>590</v>
       </c>
       <c r="H24" s="1">
-        <v>0.6745762711864407</v>
+        <v>0.67627118644067796</v>
       </c>
       <c r="I24" s="1">
-        <v>0.3254237288135593</v>
+        <v>0.32372881355932204</v>
       </c>
       <c r="K24">
-        <v>34502</v>
+        <v>34621</v>
       </c>
       <c r="L24">
-        <v>9811</v>
+        <v>9692</v>
       </c>
       <c r="M24">
         <v>44313</v>
       </c>
       <c r="O24" s="1">
-        <v>0.77859770270575224</v>
+        <v>0.78128314490104489</v>
       </c>
       <c r="P24" s="1">
-        <v>0.22140229729424774</v>
+        <v>0.21871685509895517</v>
       </c>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
@@ -1872,34 +1873,34 @@
         <v>33</v>
       </c>
       <c r="D29">
-        <v>2412</v>
+        <v>2414</v>
       </c>
       <c r="E29">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="F29">
         <v>3110</v>
       </c>
       <c r="H29" s="1">
-        <v>0.7755627009646302</v>
+        <v>0.77620578778135052</v>
       </c>
       <c r="I29" s="1">
-        <v>0.22443729903536977</v>
+        <v>0.22379421221864951</v>
       </c>
       <c r="K29">
-        <v>229278</v>
+        <v>229388</v>
       </c>
       <c r="L29">
-        <v>39151</v>
+        <v>39041</v>
       </c>
       <c r="M29">
         <v>268429</v>
       </c>
       <c r="O29" s="1">
-        <v>0.85414765170678275</v>
+        <v>0.85455744349530038</v>
       </c>
       <c r="P29" s="1">
-        <v>0.14585234829321719</v>
+        <v>0.14544255650469956</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
@@ -1977,34 +1978,34 @@
         <v>36</v>
       </c>
       <c r="D32">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="E32">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F32">
         <v>527</v>
       </c>
       <c r="H32" s="1">
-        <v>0.66793168880455411</v>
+        <v>0.66982922201138517</v>
       </c>
       <c r="I32" s="1">
-        <v>0.33206831119544594</v>
+        <v>0.33017077798861483</v>
       </c>
       <c r="K32">
-        <v>35984</v>
+        <v>35996</v>
       </c>
       <c r="L32">
-        <v>8843</v>
+        <v>8831</v>
       </c>
       <c r="M32">
         <v>44827</v>
       </c>
       <c r="O32" s="1">
-        <v>0.80273049724496393</v>
+        <v>0.80299819305329379</v>
       </c>
       <c r="P32" s="1">
-        <v>0.19726950275503602</v>
+        <v>0.19700180694670621</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
@@ -2012,34 +2013,34 @@
         <v>37</v>
       </c>
       <c r="D33">
-        <v>599</v>
+        <v>649</v>
       </c>
       <c r="E33">
-        <v>472</v>
+        <v>422</v>
       </c>
       <c r="F33">
         <v>1071</v>
       </c>
       <c r="H33" s="1">
-        <v>0.5592903828197946</v>
+        <v>0.6059757236227824</v>
       </c>
       <c r="I33" s="1">
-        <v>0.4407096171802054</v>
+        <v>0.39402427637721754</v>
       </c>
       <c r="K33">
-        <v>51698</v>
+        <v>55647</v>
       </c>
       <c r="L33">
-        <v>24691</v>
+        <v>20742</v>
       </c>
       <c r="M33">
         <v>76389</v>
       </c>
       <c r="O33" s="1">
-        <v>0.676772833784969</v>
+        <v>0.72846875859089655</v>
       </c>
       <c r="P33" s="1">
-        <v>0.32322716621503095</v>
+        <v>0.2715312414091034</v>
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
@@ -2117,34 +2118,34 @@
         <v>40</v>
       </c>
       <c r="D36">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="E36">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F36">
         <v>821</v>
       </c>
       <c r="H36" s="1">
-        <v>0.79902557856272838</v>
+        <v>0.80146163215590738</v>
       </c>
       <c r="I36" s="1">
-        <v>0.20097442143727162</v>
+        <v>0.19853836784409257</v>
       </c>
       <c r="K36">
-        <v>58403</v>
+        <v>58524</v>
       </c>
       <c r="L36">
-        <v>6432</v>
+        <v>6311</v>
       </c>
       <c r="M36">
         <v>64835</v>
       </c>
       <c r="O36" s="1">
-        <v>0.90079432405336624</v>
+        <v>0.90266059998457626</v>
       </c>
       <c r="P36" s="1">
-        <v>9.9205675946633765E-2</v>
+        <v>9.7339400015423766E-2</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
@@ -2257,34 +2258,34 @@
         <v>44</v>
       </c>
       <c r="D40">
-        <v>501</v>
+        <v>510</v>
       </c>
       <c r="E40">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="F40">
         <v>670</v>
       </c>
       <c r="H40" s="1">
-        <v>0.74776119402985075</v>
+        <v>0.76119402985074625</v>
       </c>
       <c r="I40" s="1">
-        <v>0.25223880597014925</v>
+        <v>0.23880597014925373</v>
       </c>
       <c r="K40">
-        <v>43261</v>
+        <v>43786</v>
       </c>
       <c r="L40">
-        <v>5804</v>
+        <v>5279</v>
       </c>
       <c r="M40">
         <v>49065</v>
       </c>
       <c r="O40" s="1">
-        <v>0.8817079384489962</v>
+        <v>0.89240803016406811</v>
       </c>
       <c r="P40" s="1">
-        <v>0.11829206155100377</v>
+        <v>0.10759196983593193</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
@@ -2292,34 +2293,34 @@
         <v>45</v>
       </c>
       <c r="D41">
-        <v>1154</v>
+        <v>1155</v>
       </c>
       <c r="E41">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F41">
         <v>1957</v>
       </c>
       <c r="H41" s="1">
-        <v>0.58967807869187527</v>
+        <v>0.59018906489524781</v>
       </c>
       <c r="I41" s="1">
-        <v>0.41032192130812467</v>
+        <v>0.40981093510475219</v>
       </c>
       <c r="K41">
-        <v>105943</v>
+        <v>106061</v>
       </c>
       <c r="L41">
-        <v>40676</v>
+        <v>40558</v>
       </c>
       <c r="M41">
         <v>146619</v>
       </c>
       <c r="O41" s="1">
-        <v>0.72257347274227757</v>
+        <v>0.72337827975910352</v>
       </c>
       <c r="P41" s="1">
-        <v>0.27742652725772238</v>
+        <v>0.27662172024089648</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
@@ -2397,34 +2398,34 @@
         <v>48</v>
       </c>
       <c r="D44">
-        <v>1240</v>
+        <v>1247</v>
       </c>
       <c r="E44">
-        <v>1276</v>
+        <v>1269</v>
       </c>
       <c r="F44">
         <v>2516</v>
       </c>
       <c r="H44" s="1">
-        <v>0.49284578696343401</v>
+        <v>0.49562798092209859</v>
       </c>
       <c r="I44" s="1">
-        <v>0.50715421303656594</v>
+        <v>0.50437201907790141</v>
       </c>
       <c r="K44">
-        <v>114402</v>
+        <v>115038</v>
       </c>
       <c r="L44">
-        <v>71228</v>
+        <v>70592</v>
       </c>
       <c r="M44">
         <v>185630</v>
       </c>
       <c r="O44" s="1">
-        <v>0.61629047029036255</v>
+        <v>0.61971664062920861</v>
       </c>
       <c r="P44" s="1">
-        <v>0.38370952970963745</v>
+        <v>0.38028335937079139</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
@@ -2432,34 +2433,34 @@
         <v>49</v>
       </c>
       <c r="D45">
-        <v>1195</v>
+        <v>1294</v>
       </c>
       <c r="E45">
-        <v>904</v>
+        <v>805</v>
       </c>
       <c r="F45">
         <v>2099</v>
       </c>
       <c r="H45" s="1">
-        <v>0.56931872320152455</v>
+        <v>0.61648404001905666</v>
       </c>
       <c r="I45" s="1">
-        <v>0.43068127679847545</v>
+        <v>0.38351595998094329</v>
       </c>
       <c r="K45">
-        <v>108893</v>
+        <v>116968</v>
       </c>
       <c r="L45">
-        <v>52481</v>
+        <v>44406</v>
       </c>
       <c r="M45">
         <v>161374</v>
       </c>
       <c r="O45" s="1">
-        <v>0.67478652075303336</v>
+        <v>0.72482556049921298</v>
       </c>
       <c r="P45" s="1">
-        <v>0.3252134792469667</v>
+        <v>0.27517443950078702</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
@@ -2467,34 +2468,34 @@
         <v>50</v>
       </c>
       <c r="D46">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E46">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F46">
         <v>686</v>
       </c>
       <c r="H46" s="1">
-        <v>0.7711370262390671</v>
+        <v>0.77405247813411082</v>
       </c>
       <c r="I46" s="1">
-        <v>0.22886297376093295</v>
+        <v>0.22594752186588921</v>
       </c>
       <c r="K46">
-        <v>47314</v>
+        <v>47494</v>
       </c>
       <c r="L46">
-        <v>6668</v>
+        <v>6488</v>
       </c>
       <c r="M46">
         <v>53982</v>
       </c>
       <c r="O46" s="1">
-        <v>0.87647734429995183</v>
+        <v>0.87981178911489011</v>
       </c>
       <c r="P46" s="1">
-        <v>0.12352265570004817</v>
+        <v>0.12018821088510985</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
@@ -2502,34 +2503,34 @@
         <v>51</v>
       </c>
       <c r="D47">
-        <v>533</v>
+        <v>588</v>
       </c>
       <c r="E47">
-        <v>290</v>
+        <v>235</v>
       </c>
       <c r="F47">
         <v>823</v>
       </c>
       <c r="H47" s="1">
-        <v>0.64763061968408264</v>
+        <v>0.71445929526123941</v>
       </c>
       <c r="I47" s="1">
-        <v>0.35236938031591736</v>
+        <v>0.28554070473876064</v>
       </c>
       <c r="K47">
-        <v>47370</v>
+        <v>50958</v>
       </c>
       <c r="L47">
-        <v>15300</v>
+        <v>11712</v>
       </c>
       <c r="M47">
         <v>62670</v>
       </c>
       <c r="O47" s="1">
-        <v>0.75586404978458588</v>
+        <v>0.81311632359980857</v>
       </c>
       <c r="P47" s="1">
-        <v>0.24413595021541407</v>
+        <v>0.18688367640019149</v>
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
@@ -2572,34 +2573,34 @@
         <v>53</v>
       </c>
       <c r="D49">
-        <v>454</v>
+        <v>549</v>
       </c>
       <c r="E49">
-        <v>223</v>
+        <v>128</v>
       </c>
       <c r="F49">
         <v>677</v>
       </c>
       <c r="H49" s="1">
-        <v>0.67060561299852295</v>
+        <v>0.81093057607090102</v>
       </c>
       <c r="I49" s="1">
-        <v>0.32939438700147711</v>
+        <v>0.18906942392909898</v>
       </c>
       <c r="K49">
-        <v>41757</v>
+        <v>49105</v>
       </c>
       <c r="L49">
-        <v>12435</v>
+        <v>5087</v>
       </c>
       <c r="M49">
         <v>54192</v>
       </c>
       <c r="O49" s="1">
-        <v>0.77053808680248004</v>
+        <v>0.90613005609684083</v>
       </c>
       <c r="P49" s="1">
-        <v>0.22946191319751993</v>
+        <v>9.3869943903159142E-2</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -2749,37 +2750,37 @@
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
       <c r="D54" s="13">
-        <v>32528</v>
+        <v>33208</v>
       </c>
       <c r="E54" s="13">
-        <v>14585</v>
+        <v>13905</v>
       </c>
       <c r="F54" s="13">
         <v>47113</v>
       </c>
       <c r="G54" s="13"/>
       <c r="H54" s="14">
-        <v>0.69042514804830935</v>
+        <v>0.70485853161547773</v>
       </c>
       <c r="I54" s="14">
-        <v>0.3095748519516906</v>
+        <v>0.29514146838452232</v>
       </c>
       <c r="J54" s="13"/>
       <c r="K54" s="13">
-        <v>2995426</v>
+        <v>3049248</v>
       </c>
       <c r="L54" s="13">
-        <v>745288</v>
+        <v>691466</v>
       </c>
       <c r="M54" s="13">
         <v>3740714</v>
       </c>
       <c r="N54" s="13"/>
       <c r="O54" s="14">
-        <v>0.80076316981196638</v>
+        <v>0.8151513320718986</v>
       </c>
       <c r="P54" s="14">
-        <v>0.19923683018803362</v>
+        <v>0.18484866792810142</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -2860,34 +2861,34 @@
         <v>62</v>
       </c>
       <c r="D57">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E57">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F57">
         <v>242</v>
       </c>
       <c r="H57" s="1">
-        <v>0.70661157024793386</v>
+        <v>0.71487603305785119</v>
       </c>
       <c r="I57" s="1">
-        <v>0.29338842975206614</v>
+        <v>0.28512396694214875</v>
       </c>
       <c r="K57">
-        <v>15546</v>
+        <v>15702</v>
       </c>
       <c r="L57">
-        <v>3440</v>
+        <v>3284</v>
       </c>
       <c r="M57">
         <v>18986</v>
       </c>
       <c r="O57" s="1">
-        <v>0.81881386284630786</v>
+        <v>0.82703044348467292</v>
       </c>
       <c r="P57" s="1">
-        <v>0.18118613715369219</v>
+        <v>0.17296955651532708</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -2930,34 +2931,34 @@
         <v>64</v>
       </c>
       <c r="D59">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="E59">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="F59">
         <v>163</v>
       </c>
       <c r="H59" s="1">
-        <v>0.6380368098159509</v>
+        <v>0.70552147239263807</v>
       </c>
       <c r="I59" s="1">
-        <v>0.3619631901840491</v>
+        <v>0.29447852760736198</v>
       </c>
       <c r="K59">
-        <v>9756</v>
+        <v>10452</v>
       </c>
       <c r="L59">
-        <v>3954</v>
+        <v>3258</v>
       </c>
       <c r="M59">
         <v>13710</v>
       </c>
       <c r="O59" s="1">
-        <v>0.71159737417943103</v>
+        <v>0.76236323851203502</v>
       </c>
       <c r="P59" s="1">
-        <v>0.28840262582056891</v>
+        <v>0.23763676148796498</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3002,37 +3003,37 @@
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
       <c r="D61" s="13">
-        <v>715</v>
+        <v>728</v>
       </c>
       <c r="E61" s="13">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="F61" s="13">
         <v>943</v>
       </c>
       <c r="G61" s="13"/>
       <c r="H61" s="14">
-        <v>0.7582184517497349</v>
+        <v>0.77200424178154825</v>
       </c>
       <c r="I61" s="14">
-        <v>0.2417815482502651</v>
+        <v>0.22799575821845175</v>
       </c>
       <c r="J61" s="13"/>
       <c r="K61" s="13">
-        <v>63749</v>
+        <v>64601</v>
       </c>
       <c r="L61" s="13">
-        <v>11810</v>
+        <v>10958</v>
       </c>
       <c r="M61" s="13">
         <v>75559</v>
       </c>
       <c r="N61" s="13"/>
       <c r="O61" s="14">
-        <v>0.84369830198917406</v>
+        <v>0.85497425852644948</v>
       </c>
       <c r="P61" s="14">
-        <v>0.15630169801082597</v>
+        <v>0.14502574147355046</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -3996,34 +3997,34 @@
         <v>95</v>
       </c>
       <c r="D89">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="E89">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F89">
         <v>155</v>
       </c>
       <c r="H89" s="1">
-        <v>0.67096774193548392</v>
+        <v>0.72258064516129028</v>
       </c>
       <c r="I89" s="1">
-        <v>0.32903225806451614</v>
+        <v>0.27741935483870966</v>
       </c>
       <c r="K89">
-        <v>9956</v>
+        <v>10390</v>
       </c>
       <c r="L89">
-        <v>2520</v>
+        <v>2086</v>
       </c>
       <c r="M89">
         <v>12476</v>
       </c>
       <c r="O89" s="1">
-        <v>0.79801218339211288</v>
+        <v>0.83279897403013792</v>
       </c>
       <c r="P89" s="1">
-        <v>0.20198781660788714</v>
+        <v>0.16720102596986214</v>
       </c>
     </row>
     <row r="90" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4033,37 +4034,37 @@
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
       <c r="D90" s="13">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="E90" s="13">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F90" s="13">
         <v>155</v>
       </c>
       <c r="G90" s="13"/>
       <c r="H90" s="14">
-        <v>0.67096774193548392</v>
+        <v>0.72258064516129028</v>
       </c>
       <c r="I90" s="14">
-        <v>0.32903225806451614</v>
+        <v>0.27741935483870966</v>
       </c>
       <c r="J90" s="13"/>
       <c r="K90" s="13">
-        <v>9956</v>
+        <v>10390</v>
       </c>
       <c r="L90" s="13">
-        <v>2520</v>
+        <v>2086</v>
       </c>
       <c r="M90" s="13">
         <v>12476</v>
       </c>
       <c r="N90" s="13"/>
       <c r="O90" s="14">
-        <v>0.79801218339211288</v>
+        <v>0.83279897403013792</v>
       </c>
       <c r="P90" s="14">
-        <v>0.20198781660788714</v>
+        <v>0.16720102596986214</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
@@ -4144,34 +4145,34 @@
         <v>100</v>
       </c>
       <c r="D93">
-        <v>627</v>
+        <v>711</v>
       </c>
       <c r="E93">
-        <v>276</v>
+        <v>192</v>
       </c>
       <c r="F93">
         <v>903</v>
       </c>
       <c r="H93" s="1">
-        <v>0.69435215946843853</v>
+        <v>0.78737541528239208</v>
       </c>
       <c r="I93" s="1">
-        <v>0.30564784053156147</v>
+        <v>0.21262458471760798</v>
       </c>
       <c r="K93">
-        <v>59463</v>
+        <v>66838</v>
       </c>
       <c r="L93">
-        <v>16018</v>
+        <v>8643</v>
       </c>
       <c r="M93">
         <v>75481</v>
       </c>
       <c r="O93" s="1">
-        <v>0.78778765517150007</v>
+        <v>0.88549436281978244</v>
       </c>
       <c r="P93" s="1">
-        <v>0.21221234482849988</v>
+        <v>0.11450563718021754</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
@@ -4564,34 +4565,34 @@
         <v>112</v>
       </c>
       <c r="D105">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E105">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F105">
         <v>145</v>
       </c>
       <c r="H105" s="1">
-        <v>0.77241379310344827</v>
+        <v>0.78620689655172415</v>
       </c>
       <c r="I105" s="1">
-        <v>0.22758620689655173</v>
+        <v>0.21379310344827587</v>
       </c>
       <c r="K105">
-        <v>10725</v>
+        <v>10857</v>
       </c>
       <c r="L105">
-        <v>1880</v>
+        <v>1748</v>
       </c>
       <c r="M105">
         <v>12605</v>
       </c>
       <c r="O105" s="1">
-        <v>0.85085283617612062</v>
+        <v>0.86132487108290356</v>
       </c>
       <c r="P105" s="1">
-        <v>0.14914716382387941</v>
+        <v>0.13867512891709638</v>
       </c>
     </row>
     <row r="106" spans="2:16" x14ac:dyDescent="0.25">
@@ -4704,34 +4705,34 @@
         <v>116</v>
       </c>
       <c r="D109">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="E109">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F109">
         <v>529</v>
       </c>
       <c r="H109" s="1">
-        <v>0.86389413988657848</v>
+        <v>0.87334593572778829</v>
       </c>
       <c r="I109" s="1">
-        <v>0.13610586011342155</v>
+        <v>0.12665406427221171</v>
       </c>
       <c r="K109">
-        <v>43669</v>
+        <v>44125</v>
       </c>
       <c r="L109">
-        <v>2832</v>
+        <v>2376</v>
       </c>
       <c r="M109">
         <v>46501</v>
       </c>
       <c r="O109" s="1">
-        <v>0.93909808391217398</v>
+        <v>0.94890432463817986</v>
       </c>
       <c r="P109" s="1">
-        <v>6.0901916087826066E-2</v>
+        <v>5.1095675361820178E-2</v>
       </c>
     </row>
     <row r="110" spans="2:16" x14ac:dyDescent="0.25">
@@ -4879,34 +4880,34 @@
         <v>121</v>
       </c>
       <c r="D114">
-        <v>661</v>
+        <v>734</v>
       </c>
       <c r="E114">
-        <v>300</v>
+        <v>227</v>
       </c>
       <c r="F114">
         <v>961</v>
       </c>
       <c r="H114" s="1">
-        <v>0.68782518210197707</v>
+        <v>0.76378772112382931</v>
       </c>
       <c r="I114" s="1">
-        <v>0.31217481789802287</v>
+        <v>0.23621227887617066</v>
       </c>
       <c r="K114">
-        <v>59756</v>
+        <v>64643</v>
       </c>
       <c r="L114">
-        <v>15718</v>
+        <v>10831</v>
       </c>
       <c r="M114">
         <v>75474</v>
       </c>
       <c r="O114" s="1">
-        <v>0.79174285184301874</v>
+        <v>0.85649362694437825</v>
       </c>
       <c r="P114" s="1">
-        <v>0.20825714815698121</v>
+        <v>0.14350637305562181</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
@@ -4949,34 +4950,34 @@
         <v>123</v>
       </c>
       <c r="D116">
-        <v>354</v>
+        <v>380</v>
       </c>
       <c r="E116">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="F116">
         <v>496</v>
       </c>
       <c r="H116" s="1">
-        <v>0.71370967741935487</v>
+        <v>0.7661290322580645</v>
       </c>
       <c r="I116" s="1">
-        <v>0.28629032258064518</v>
+        <v>0.23387096774193547</v>
       </c>
       <c r="K116">
-        <v>30345</v>
+        <v>32105</v>
       </c>
       <c r="L116">
-        <v>5848</v>
+        <v>4088</v>
       </c>
       <c r="M116">
         <v>36193</v>
       </c>
       <c r="O116" s="1">
-        <v>0.83842179426961017</v>
+        <v>0.88704998204072616</v>
       </c>
       <c r="P116" s="1">
-        <v>0.16157820573038986</v>
+        <v>0.1129500179592739</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
@@ -5231,37 +5232,37 @@
       <c r="B124" s="13"/>
       <c r="C124" s="13"/>
       <c r="D124" s="13">
-        <v>8319</v>
+        <v>8509</v>
       </c>
       <c r="E124" s="13">
-        <v>2115</v>
+        <v>1925</v>
       </c>
       <c r="F124" s="13">
         <v>10434</v>
       </c>
       <c r="G124" s="13"/>
       <c r="H124" s="14">
-        <v>0.79729729729729726</v>
+        <v>0.81550699635806023</v>
       </c>
       <c r="I124" s="14">
-        <v>0.20270270270270271</v>
+        <v>0.18449300364193982</v>
       </c>
       <c r="J124" s="13"/>
       <c r="K124" s="13">
-        <v>767268</v>
+        <v>781878</v>
       </c>
       <c r="L124" s="13">
-        <v>102354</v>
+        <v>87744</v>
       </c>
       <c r="M124" s="13">
         <v>869622</v>
       </c>
       <c r="N124" s="13"/>
       <c r="O124" s="14">
-        <v>0.88230058577174908</v>
+        <v>0.89910098870543753</v>
       </c>
       <c r="P124" s="14">
-        <v>0.11769941422825089</v>
+        <v>0.10089901129456247</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
@@ -5587,34 +5588,34 @@
         <v>142</v>
       </c>
       <c r="D134">
-        <v>287</v>
+        <v>320</v>
       </c>
       <c r="E134">
-        <v>144</v>
+        <v>111</v>
       </c>
       <c r="F134">
         <v>431</v>
       </c>
       <c r="H134" s="1">
-        <v>0.66589327146171695</v>
+        <v>0.74245939675174011</v>
       </c>
       <c r="I134" s="1">
-        <v>0.33410672853828305</v>
+        <v>0.25754060324825984</v>
       </c>
       <c r="K134">
-        <v>26810</v>
+        <v>29353</v>
       </c>
       <c r="L134">
-        <v>7101</v>
+        <v>4558</v>
       </c>
       <c r="M134">
         <v>33911</v>
       </c>
       <c r="O134" s="1">
-        <v>0.79059892070419624</v>
+        <v>0.86558933679337091</v>
       </c>
       <c r="P134" s="1">
-        <v>0.20940107929580373</v>
+        <v>0.13441066320662912</v>
       </c>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
@@ -5729,37 +5730,37 @@
       <c r="B138" s="13"/>
       <c r="C138" s="13"/>
       <c r="D138" s="13">
-        <v>3713</v>
+        <v>3746</v>
       </c>
       <c r="E138" s="13">
-        <v>1260</v>
+        <v>1227</v>
       </c>
       <c r="F138" s="13">
         <v>4973</v>
       </c>
       <c r="G138" s="13"/>
       <c r="H138" s="14">
-        <v>0.74663181178363158</v>
+        <v>0.75326764528453649</v>
       </c>
       <c r="I138" s="14">
-        <v>0.25336818821636836</v>
+        <v>0.24673235471546351</v>
       </c>
       <c r="J138" s="13"/>
       <c r="K138" s="13">
-        <v>342404</v>
+        <v>344947</v>
       </c>
       <c r="L138" s="13">
-        <v>57936</v>
+        <v>55393</v>
       </c>
       <c r="M138" s="13">
         <v>400340</v>
       </c>
       <c r="N138" s="13"/>
       <c r="O138" s="14">
-        <v>0.85528300944197433</v>
+        <v>0.86163511015636707</v>
       </c>
       <c r="P138" s="14">
-        <v>0.14471699055802567</v>
+        <v>0.1383648898436329</v>
       </c>
     </row>
     <row r="139" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5769,37 +5770,37 @@
       <c r="B139" s="13"/>
       <c r="C139" s="13"/>
       <c r="D139" s="13">
-        <v>46371</v>
+        <v>47314</v>
       </c>
       <c r="E139" s="13">
-        <v>19642</v>
+        <v>18699</v>
       </c>
       <c r="F139" s="13">
         <v>66013</v>
       </c>
       <c r="G139" s="13"/>
       <c r="H139" s="14">
-        <v>0.70245254722554651</v>
+        <v>0.71673761228848865</v>
       </c>
       <c r="I139" s="14">
-        <v>0.29754745277445349</v>
+        <v>0.28326238771151135</v>
       </c>
       <c r="J139" s="13"/>
       <c r="K139" s="13">
-        <v>4268320</v>
+        <v>4342136</v>
       </c>
       <c r="L139" s="13">
-        <v>1007617</v>
+        <v>933801</v>
       </c>
       <c r="M139" s="13">
         <v>5275937</v>
       </c>
       <c r="N139" s="13"/>
       <c r="O139" s="14">
-        <v>0.80901648370706469</v>
+        <v>0.82300755297115946</v>
       </c>
       <c r="P139" s="14">
-        <v>0.19098351629293525</v>
+        <v>0.17699244702884057</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to county stats
</commit_message>
<xml_diff>
--- a/Locations/CountyStats.xlsx
+++ b/Locations/CountyStats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Git\Rainfall\DQ_Checks\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7FF8C0A-0C3B-43BB-A124-C511AA818422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C763CAD4-68AD-4499-88A5-CE8BCFAF1C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{59BE05DA-B4D5-4FF3-A30D-5F4B640329E8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4C951E89-C97B-4EDB-ACEA-1B46BBF1DBAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -889,26 +889,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{999D7B3C-0CD7-4052-A782-446FAA4B0CE9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C283B2D-D1BA-4899-8D74-89BD76215796}">
   <dimension ref="A1:P139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
     <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8.28515625" style="12" bestFit="1" customWidth="1"/>
@@ -1278,34 +1278,34 @@
         <v>16</v>
       </c>
       <c r="D12">
-        <v>426</v>
+        <v>480</v>
       </c>
       <c r="E12">
-        <v>148</v>
+        <v>94</v>
       </c>
       <c r="F12">
         <v>574</v>
       </c>
       <c r="H12" s="12">
-        <v>0.74216027874564461</v>
+        <v>0.83623693379790942</v>
       </c>
       <c r="I12" s="12">
-        <v>0.25783972125435539</v>
+        <v>0.16376306620209058</v>
       </c>
       <c r="K12">
-        <v>37760</v>
+        <v>40912</v>
       </c>
       <c r="L12">
-        <v>6101</v>
+        <v>2949</v>
       </c>
       <c r="M12">
         <v>43861</v>
       </c>
       <c r="O12" s="12">
-        <v>0.86090148423428559</v>
+        <v>0.93276487084197812</v>
       </c>
       <c r="P12" s="12">
-        <v>0.13909851576571441</v>
+        <v>6.7235129158021933E-2</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1351,31 +1351,31 @@
         <v>918</v>
       </c>
       <c r="E14">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F14">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="H14" s="12">
-        <v>0.82926829268292679</v>
+        <v>0.83001808318264014</v>
       </c>
       <c r="I14" s="12">
-        <v>0.17073170731707318</v>
+        <v>0.16998191681735986</v>
       </c>
       <c r="K14">
         <v>84763</v>
       </c>
       <c r="L14">
-        <v>7596</v>
+        <v>7531</v>
       </c>
       <c r="M14">
-        <v>92359</v>
+        <v>92294</v>
       </c>
       <c r="O14" s="12">
-        <v>0.91775571411557078</v>
+        <v>0.91840206297267424</v>
       </c>
       <c r="P14" s="12">
-        <v>8.2244285884429238E-2</v>
+        <v>8.159793702732572E-2</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -1593,34 +1593,34 @@
         <v>25</v>
       </c>
       <c r="D21">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="E21">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F21">
         <v>1290</v>
       </c>
       <c r="H21" s="12">
-        <v>0.8046511627906977</v>
+        <v>0.8054263565891473</v>
       </c>
       <c r="I21" s="12">
-        <v>0.19534883720930232</v>
+        <v>0.1945736434108527</v>
       </c>
       <c r="K21">
-        <v>92905</v>
+        <v>92929</v>
       </c>
       <c r="L21">
-        <v>8578</v>
+        <v>8554</v>
       </c>
       <c r="M21">
         <v>101483</v>
       </c>
       <c r="O21" s="12">
-        <v>0.91547352758590106</v>
+        <v>0.91571002039750504</v>
       </c>
       <c r="P21" s="12">
-        <v>8.4526472414098913E-2</v>
+        <v>8.4289979602494999E-2</v>
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
@@ -1628,34 +1628,34 @@
         <v>26</v>
       </c>
       <c r="D22">
-        <v>854</v>
+        <v>1017</v>
       </c>
       <c r="E22">
-        <v>325</v>
+        <v>162</v>
       </c>
       <c r="F22">
         <v>1179</v>
       </c>
       <c r="H22" s="12">
-        <v>0.72434266327396102</v>
+        <v>0.86259541984732824</v>
       </c>
       <c r="I22" s="12">
-        <v>0.27565733672603904</v>
+        <v>0.13740458015267176</v>
       </c>
       <c r="K22">
-        <v>79157</v>
+        <v>89974</v>
       </c>
       <c r="L22">
-        <v>16455</v>
+        <v>5638</v>
       </c>
       <c r="M22">
         <v>95612</v>
       </c>
       <c r="O22" s="12">
-        <v>0.82789817177760117</v>
+        <v>0.94103250637995228</v>
       </c>
       <c r="P22" s="12">
-        <v>0.17210182822239886</v>
+        <v>5.896749362004769E-2</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
@@ -1663,34 +1663,34 @@
         <v>27</v>
       </c>
       <c r="D23">
-        <v>1184</v>
+        <v>1186</v>
       </c>
       <c r="E23">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F23">
         <v>1720</v>
       </c>
       <c r="H23" s="12">
-        <v>0.68837209302325586</v>
+        <v>0.68953488372093019</v>
       </c>
       <c r="I23" s="12">
-        <v>0.3116279069767442</v>
+        <v>0.31046511627906975</v>
       </c>
       <c r="K23">
-        <v>105408</v>
+        <v>105564</v>
       </c>
       <c r="L23">
-        <v>25651</v>
+        <v>25495</v>
       </c>
       <c r="M23">
         <v>131059</v>
       </c>
       <c r="O23" s="12">
-        <v>0.80427898885234894</v>
+        <v>0.80546929245606935</v>
       </c>
       <c r="P23" s="12">
-        <v>0.19572101114765106</v>
+        <v>0.19453070754393059</v>
       </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
@@ -1838,34 +1838,34 @@
         <v>32</v>
       </c>
       <c r="D28">
-        <v>1549</v>
+        <v>1762</v>
       </c>
       <c r="E28">
-        <v>675</v>
+        <v>462</v>
       </c>
       <c r="F28">
         <v>2224</v>
       </c>
       <c r="H28" s="12">
-        <v>0.69649280575539574</v>
+        <v>0.79226618705035967</v>
       </c>
       <c r="I28" s="12">
-        <v>0.30350719424460432</v>
+        <v>0.2077338129496403</v>
       </c>
       <c r="K28">
-        <v>141193</v>
+        <v>155146</v>
       </c>
       <c r="L28">
-        <v>30141</v>
+        <v>16188</v>
       </c>
       <c r="M28">
         <v>171334</v>
       </c>
       <c r="O28" s="12">
-        <v>0.82408045104882865</v>
+        <v>0.9055178773623449</v>
       </c>
       <c r="P28" s="12">
-        <v>0.1759195489511714</v>
+        <v>9.4482122637655111E-2</v>
       </c>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
@@ -1873,34 +1873,34 @@
         <v>33</v>
       </c>
       <c r="D29">
-        <v>2543</v>
+        <v>2670</v>
       </c>
       <c r="E29">
-        <v>568</v>
+        <v>442</v>
       </c>
       <c r="F29">
-        <v>3111</v>
+        <v>3112</v>
       </c>
       <c r="H29" s="12">
-        <v>0.81742205078752816</v>
+        <v>0.85796915167095111</v>
       </c>
       <c r="I29" s="12">
-        <v>0.18257794921247186</v>
+        <v>0.14203084832904883</v>
       </c>
       <c r="K29">
-        <v>238462</v>
+        <v>248104</v>
       </c>
       <c r="L29">
-        <v>29979</v>
+        <v>20402</v>
       </c>
       <c r="M29">
-        <v>268441</v>
+        <v>268506</v>
       </c>
       <c r="O29" s="12">
-        <v>0.8883218286327349</v>
+        <v>0.92401659553231585</v>
       </c>
       <c r="P29" s="12">
-        <v>0.11167817136726506</v>
+        <v>7.5983404467684146E-2</v>
       </c>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
@@ -1978,34 +1978,34 @@
         <v>36</v>
       </c>
       <c r="D32">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E32">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F32">
         <v>527</v>
       </c>
       <c r="H32" s="12">
-        <v>0.68880455407969643</v>
+        <v>0.69259962049335866</v>
       </c>
       <c r="I32" s="12">
-        <v>0.31119544592030363</v>
+        <v>0.30740037950664134</v>
       </c>
       <c r="K32">
-        <v>36726</v>
+        <v>36846</v>
       </c>
       <c r="L32">
-        <v>8101</v>
+        <v>7981</v>
       </c>
       <c r="M32">
         <v>44827</v>
       </c>
       <c r="O32" s="12">
-        <v>0.81928302139335674</v>
+        <v>0.82195997947665467</v>
       </c>
       <c r="P32" s="12">
-        <v>0.18071697860664332</v>
+        <v>0.1780400205233453</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
@@ -2048,34 +2048,34 @@
         <v>38</v>
       </c>
       <c r="D34">
-        <v>923</v>
+        <v>926</v>
       </c>
       <c r="E34">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F34">
         <v>1141</v>
       </c>
       <c r="H34" s="12">
-        <v>0.80893952673093772</v>
+        <v>0.81156879929886061</v>
       </c>
       <c r="I34" s="12">
-        <v>0.19106047326906223</v>
+        <v>0.18843120070113936</v>
       </c>
       <c r="K34">
-        <v>79408</v>
+        <v>79708</v>
       </c>
       <c r="L34">
-        <v>8030</v>
+        <v>7730</v>
       </c>
       <c r="M34">
         <v>87438</v>
       </c>
       <c r="O34" s="12">
-        <v>0.90816349870765567</v>
+        <v>0.91159450124659758</v>
       </c>
       <c r="P34" s="12">
-        <v>9.1836501292344289E-2</v>
+        <v>8.8405498753402409E-2</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
@@ -2083,34 +2083,34 @@
         <v>39</v>
       </c>
       <c r="D35">
-        <v>567</v>
+        <v>656</v>
       </c>
       <c r="E35">
-        <v>217</v>
+        <v>128</v>
       </c>
       <c r="F35">
         <v>784</v>
       </c>
       <c r="H35" s="12">
-        <v>0.7232142857142857</v>
+        <v>0.83673469387755106</v>
       </c>
       <c r="I35" s="12">
-        <v>0.2767857142857143</v>
+        <v>0.16326530612244897</v>
       </c>
       <c r="K35">
-        <v>52184</v>
+        <v>58016</v>
       </c>
       <c r="L35">
-        <v>10407</v>
+        <v>4575</v>
       </c>
       <c r="M35">
         <v>62591</v>
       </c>
       <c r="O35" s="12">
-        <v>0.83373008899042989</v>
+        <v>0.92690642424629743</v>
       </c>
       <c r="P35" s="12">
-        <v>0.16626991100957006</v>
+        <v>7.3093575753702608E-2</v>
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
@@ -2188,34 +2188,34 @@
         <v>42</v>
       </c>
       <c r="D38">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="E38">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F38">
         <v>760</v>
       </c>
       <c r="H38" s="12">
-        <v>0.76447368421052631</v>
+        <v>0.76578947368421058</v>
       </c>
       <c r="I38" s="12">
-        <v>0.23552631578947369</v>
+        <v>0.23421052631578948</v>
       </c>
       <c r="K38">
-        <v>50563</v>
+        <v>50599</v>
       </c>
       <c r="L38">
-        <v>4721</v>
+        <v>4685</v>
       </c>
       <c r="M38">
         <v>55284</v>
       </c>
       <c r="O38" s="12">
-        <v>0.91460458722234284</v>
+        <v>0.9152557702047609</v>
       </c>
       <c r="P38" s="12">
-        <v>8.5395412777657193E-2</v>
+        <v>8.4744229795239129E-2</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
@@ -2363,34 +2363,34 @@
         <v>47</v>
       </c>
       <c r="D43">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="E43">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F43">
         <v>837</v>
       </c>
       <c r="H43" s="12">
-        <v>0.85782556750298689</v>
+        <v>0.85902031063321382</v>
       </c>
       <c r="I43" s="12">
-        <v>0.14217443249701314</v>
+        <v>0.14097968936678615</v>
       </c>
       <c r="K43">
-        <v>60814</v>
+        <v>60933</v>
       </c>
       <c r="L43">
-        <v>3180</v>
+        <v>3061</v>
       </c>
       <c r="M43">
         <v>63994</v>
       </c>
       <c r="O43" s="12">
-        <v>0.95030784136012747</v>
+        <v>0.95216739069287748</v>
       </c>
       <c r="P43" s="12">
-        <v>4.9692158639872488E-2</v>
+        <v>4.7832609307122541E-2</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
@@ -2398,34 +2398,34 @@
         <v>48</v>
       </c>
       <c r="D44">
-        <v>1435</v>
+        <v>1438</v>
       </c>
       <c r="E44">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="F44">
         <v>2516</v>
       </c>
       <c r="H44" s="12">
-        <v>0.57034976152623207</v>
+        <v>0.57154213036565982</v>
       </c>
       <c r="I44" s="12">
-        <v>0.42965023847376788</v>
+        <v>0.42845786963434024</v>
       </c>
       <c r="K44">
-        <v>130896</v>
+        <v>131185</v>
       </c>
       <c r="L44">
-        <v>54734</v>
+        <v>54445</v>
       </c>
       <c r="M44">
         <v>185630</v>
       </c>
       <c r="O44" s="12">
-        <v>0.70514464256855036</v>
+        <v>0.70670150298981849</v>
       </c>
       <c r="P44" s="12">
-        <v>0.29485535743144964</v>
+        <v>0.29329849701018157</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
@@ -2433,34 +2433,34 @@
         <v>49</v>
       </c>
       <c r="D45">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="E45">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F45">
         <v>2099</v>
       </c>
       <c r="H45" s="12">
-        <v>0.78799428299190089</v>
+        <v>0.78847070033349209</v>
       </c>
       <c r="I45" s="12">
-        <v>0.21200571700809909</v>
+        <v>0.21152929966650785</v>
       </c>
       <c r="K45">
-        <v>143894</v>
+        <v>144014</v>
       </c>
       <c r="L45">
-        <v>17480</v>
+        <v>17360</v>
       </c>
       <c r="M45">
         <v>161374</v>
       </c>
       <c r="O45" s="12">
-        <v>0.89168019631415218</v>
+        <v>0.89242381052709852</v>
       </c>
       <c r="P45" s="12">
-        <v>0.10831980368584779</v>
+        <v>0.10757618947290146</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
@@ -2538,34 +2538,34 @@
         <v>52</v>
       </c>
       <c r="D48">
-        <v>632</v>
+        <v>724</v>
       </c>
       <c r="E48">
-        <v>214</v>
+        <v>122</v>
       </c>
       <c r="F48">
         <v>846</v>
       </c>
       <c r="H48" s="12">
-        <v>0.74704491725768318</v>
+        <v>0.85579196217494091</v>
       </c>
       <c r="I48" s="12">
-        <v>0.25295508274231676</v>
+        <v>0.14420803782505912</v>
       </c>
       <c r="K48">
-        <v>57899</v>
+        <v>63631</v>
       </c>
       <c r="L48">
-        <v>9465</v>
+        <v>3733</v>
       </c>
       <c r="M48">
         <v>67364</v>
       </c>
       <c r="O48" s="12">
-        <v>0.85949468558874176</v>
+        <v>0.94458464461730296</v>
       </c>
       <c r="P48" s="12">
-        <v>0.14050531441125824</v>
+        <v>5.5415355382696992E-2</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
@@ -2750,37 +2750,37 @@
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
       <c r="D54" s="13">
-        <v>36101</v>
+        <v>36853</v>
       </c>
       <c r="E54" s="13">
-        <v>11012</v>
+        <v>10260</v>
       </c>
       <c r="F54" s="13">
         <v>47113</v>
       </c>
       <c r="G54" s="13"/>
       <c r="H54" s="14">
-        <v>0.76626408846815108</v>
+        <v>0.78222571264831364</v>
       </c>
       <c r="I54" s="14">
-        <v>0.23373591153184897</v>
+        <v>0.21777428735168636</v>
       </c>
       <c r="J54" s="13"/>
       <c r="K54" s="13">
-        <v>3258547</v>
+        <v>3308839</v>
       </c>
       <c r="L54" s="13">
-        <v>482167</v>
+        <v>431875</v>
       </c>
       <c r="M54" s="13">
         <v>3740714</v>
       </c>
       <c r="N54" s="13"/>
       <c r="O54" s="14">
-        <v>0.87110294986465153</v>
+        <v>0.8845474420124072</v>
       </c>
       <c r="P54" s="14">
-        <v>0.1288970501353485</v>
+        <v>0.11545255798759274</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -3919,34 +3919,34 @@
         <v>93</v>
       </c>
       <c r="D87">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E87">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F87">
         <v>113</v>
       </c>
       <c r="H87" s="12">
-        <v>0.59292035398230092</v>
+        <v>0.60176991150442483</v>
       </c>
       <c r="I87" s="12">
-        <v>0.40707964601769914</v>
+        <v>0.39823008849557523</v>
       </c>
       <c r="K87">
-        <v>5920</v>
+        <v>5944</v>
       </c>
       <c r="L87">
-        <v>2409</v>
+        <v>2385</v>
       </c>
       <c r="M87">
         <v>8329</v>
       </c>
       <c r="O87" s="12">
-        <v>0.71076960019209989</v>
+        <v>0.71365109857125708</v>
       </c>
       <c r="P87" s="12">
-        <v>0.28923039980790011</v>
+        <v>0.28634890142874292</v>
       </c>
     </row>
     <row r="88" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3956,37 +3956,37 @@
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
       <c r="D88" s="13">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="E88" s="13">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F88" s="13">
         <v>2149</v>
       </c>
       <c r="G88" s="13"/>
       <c r="H88" s="14">
-        <v>0.76733364355514189</v>
+        <v>0.76779897626803162</v>
       </c>
       <c r="I88" s="14">
-        <v>0.23266635644485809</v>
+        <v>0.23220102373196835</v>
       </c>
       <c r="J88" s="13"/>
       <c r="K88" s="13">
-        <v>137389</v>
+        <v>137413</v>
       </c>
       <c r="L88" s="13">
-        <v>22208</v>
+        <v>22184</v>
       </c>
       <c r="M88" s="13">
         <v>159597</v>
       </c>
       <c r="N88" s="13"/>
       <c r="O88" s="14">
-        <v>0.86084951471518889</v>
+        <v>0.86099989348170702</v>
       </c>
       <c r="P88" s="14">
-        <v>0.13915048528481111</v>
+        <v>0.13900010651829295</v>
       </c>
     </row>
     <row r="89" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5770,37 +5770,37 @@
       <c r="B139" s="13"/>
       <c r="C139" s="13"/>
       <c r="D139" s="13">
-        <v>51403</v>
+        <v>52156</v>
       </c>
       <c r="E139" s="13">
-        <v>14610</v>
+        <v>13857</v>
       </c>
       <c r="F139" s="13">
         <v>66013</v>
       </c>
       <c r="G139" s="13"/>
       <c r="H139" s="14">
-        <v>0.77867995697817094</v>
+        <v>0.7900868010846348</v>
       </c>
       <c r="I139" s="14">
-        <v>0.22132004302182903</v>
+        <v>0.20991319891536517</v>
       </c>
       <c r="J139" s="13"/>
       <c r="K139" s="13">
-        <v>4639567</v>
+        <v>4689883</v>
       </c>
       <c r="L139" s="13">
-        <v>636370</v>
+        <v>586054</v>
       </c>
       <c r="M139" s="13">
         <v>5275937</v>
       </c>
       <c r="N139" s="13"/>
       <c r="O139" s="14">
-        <v>0.87938256275615123</v>
+        <v>0.88891944691530622</v>
       </c>
       <c r="P139" s="14">
-        <v>0.12061743724384882</v>
+        <v>0.11108055308469376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>